<commit_message>
Added 2 new tabs -> Task, Misc tasks yet to assign
</commit_message>
<xml_diff>
--- a/docs/PM-1 Project Management/PM-1.2 Plans/PM-1.2.1 Project Plan/vms_implementation_plan_v0.1a.xlsx
+++ b/docs/PM-1 Project Management/PM-1.2 Plans/PM-1.2.1 Project Plan/vms_implementation_plan_v0.1a.xlsx
@@ -1,16 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14325" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14320" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tasks" sheetId="2" r:id="rId2"/>
+    <sheet name="Misc Tasks yet to assign" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tasks!$A$1:$N$99</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="147">
   <si>
     <t>No</t>
   </si>
@@ -286,7 +289,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Use Case Implementation</t>
@@ -312,7 +314,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Report Utility</t>
@@ -338,7 +339,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Common functionalities</t>
@@ -364,7 +364,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>User Access Control &amp; Security</t>
@@ -390,7 +389,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Solution framework</t>
@@ -398,13 +396,256 @@
   </si>
   <si>
     <t xml:space="preserve">Week </t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Sequence</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Planned Start Date</t>
+  </si>
+  <si>
+    <t>Planned End Date</t>
+  </si>
+  <si>
+    <t>Action By</t>
+  </si>
+  <si>
+    <t>Planned Review Date</t>
+  </si>
+  <si>
+    <t>Review Status</t>
+  </si>
+  <si>
+    <t>Review By</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Volunteer</t>
+  </si>
+  <si>
+    <t>Finalised ERD</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Zaw, Thida, Peishan</t>
+  </si>
+  <si>
+    <t>Data Model Specs</t>
+  </si>
+  <si>
+    <t>WIP</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Database Tables Creation</t>
+  </si>
+  <si>
+    <t>Perform reverse engineering using Rational Rose</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Register Volunteer Profile</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Update Volunteer Profile</t>
+  </si>
+  <si>
+    <t>Unit Test</t>
+  </si>
+  <si>
+    <t>Common</t>
+  </si>
+  <si>
+    <t>A &amp; A</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>ACL</t>
+  </si>
+  <si>
+    <t>Send UI Screen Shots</t>
+  </si>
+  <si>
+    <t>Base</t>
+  </si>
+  <si>
+    <t>Pagination</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Browse for Projects</t>
+  </si>
+  <si>
+    <t>Raise Interest to Project</t>
+  </si>
+  <si>
+    <t>Review Project Interest by Volunteer and Assign Volunteer to Project</t>
+  </si>
+  <si>
+    <t>Post Feedback to Project</t>
+  </si>
+  <si>
+    <t>Post Experience or Inspiration Stories</t>
+  </si>
+  <si>
+    <t>Manage Volunteer Account</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Manage Projects</t>
+  </si>
+  <si>
+    <t>Setup Project Details</t>
+  </si>
+  <si>
+    <t>Assign Roles to Project Member</t>
+  </si>
+  <si>
+    <t>Send Invitation to Volunteer</t>
+  </si>
+  <si>
+    <t>Review and Reply Project Proposal</t>
+  </si>
+  <si>
+    <t>Setup Project Calendar</t>
+  </si>
+  <si>
+    <t>Itinerary</t>
+  </si>
+  <si>
+    <t>Prepare Itinerary Plan</t>
+  </si>
+  <si>
+    <t>Submit Itinerary Plan</t>
+  </si>
+  <si>
+    <t>Review and Reply Itinerary Plan</t>
+  </si>
+  <si>
+    <t>Change to use XML for database</t>
+  </si>
+  <si>
+    <t>Certificate</t>
+  </si>
+  <si>
+    <t>Generate Certificate</t>
+  </si>
+  <si>
+    <t>Staff</t>
+  </si>
+  <si>
+    <t>Manage Staff Account</t>
+  </si>
+  <si>
+    <t>Register Staff Account</t>
+  </si>
+  <si>
+    <t>Update Profile by Staff</t>
+  </si>
+  <si>
+    <t>Populate Code Table Data</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>User Manual</t>
+  </si>
+  <si>
+    <t>Installation Guide</t>
+  </si>
+  <si>
+    <t>Operations Guide</t>
+  </si>
+  <si>
+    <t>End of Project Report</t>
+  </si>
+  <si>
+    <t>Thida, Dio</t>
+  </si>
+  <si>
+    <t>3rd Project Presentation</t>
+  </si>
+  <si>
+    <t>3rd Quality Audit</t>
+  </si>
+  <si>
+    <t>Detailed Design Specs</t>
+  </si>
+  <si>
+    <t>Draw the Jasper Report template for Certificate Management</t>
+  </si>
+  <si>
+    <t>Code Lookup</t>
+  </si>
+  <si>
+    <t>User Lookup</t>
+  </si>
+  <si>
+    <t>Email Integration</t>
+  </si>
+  <si>
+    <t>Code Lookup Class</t>
+  </si>
+  <si>
+    <t>Meeting Minutes</t>
+  </si>
+  <si>
+    <t>Timelog</t>
+  </si>
+  <si>
+    <t>Audit Log Meeting Minutes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -483,8 +724,23 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -515,8 +771,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -524,8 +786,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="263">
+  <cellStyleXfs count="267">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -789,8 +1066,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -815,8 +1096,17 @@
       <alignment horizontal="left" vertical="center" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="263">
+  <cellStyles count="267">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -948,6 +1238,8 @@
     <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1079,6 +1371,8 @@
     <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1415,22 +1709,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="5.125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="35.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="35.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="2" customWidth="1"/>
-    <col min="4" max="5" width="10.875" style="2"/>
+    <col min="4" max="5" width="10.83203125" style="2"/>
     <col min="6" max="7" width="8.5" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.875" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="10.875" style="2"/>
+    <col min="8" max="8" width="10.83203125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1447,7 +1741,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>13</v>
@@ -1460,7 +1754,7 @@
         <v>40804</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="B3" s="2" t="s">
         <v>21</v>
       </c>
@@ -1474,7 +1768,7 @@
         <v>40790</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="B4" s="2" t="s">
         <v>22</v>
       </c>
@@ -1488,7 +1782,7 @@
         <v>40790</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="B5" s="2" t="s">
         <v>23</v>
       </c>
@@ -1502,7 +1796,7 @@
         <v>40790</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
@@ -1516,7 +1810,7 @@
         <v>40790</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
@@ -1530,7 +1824,7 @@
         <v>40790</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="B8" s="2" t="s">
         <v>40</v>
       </c>
@@ -1544,7 +1838,7 @@
         <v>40796</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1558,7 +1852,7 @@
         <v>40790</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="B10" s="2" t="s">
         <v>32</v>
       </c>
@@ -1572,7 +1866,7 @@
         <v>40790</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="B11" s="2" t="s">
         <v>33</v>
       </c>
@@ -1586,7 +1880,7 @@
         <v>40790</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="5"/>
       <c r="B12" s="2" t="s">
         <v>34</v>
@@ -1601,7 +1895,7 @@
         <v>40790</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="B13" s="2" t="s">
         <v>40</v>
       </c>
@@ -1615,7 +1909,7 @@
         <v>40796</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="B14" s="2" t="s">
         <v>11</v>
       </c>
@@ -1629,7 +1923,7 @@
         <v>40790</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="B15" s="2" t="s">
         <v>16</v>
       </c>
@@ -1643,7 +1937,7 @@
         <v>40790</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="B16" s="2" t="s">
         <v>40</v>
       </c>
@@ -1657,7 +1951,7 @@
         <v>40796</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="B17" s="2" t="s">
         <v>18</v>
       </c>
@@ -1671,7 +1965,7 @@
         <v>40790</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="B18" s="2" t="s">
         <v>24</v>
       </c>
@@ -1685,7 +1979,7 @@
         <v>40790</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="B19" s="2" t="s">
         <v>25</v>
       </c>
@@ -1699,7 +1993,7 @@
         <v>40790</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="B20" s="2" t="s">
         <v>37</v>
       </c>
@@ -1713,7 +2007,7 @@
         <v>40790</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="B21" s="2" t="s">
         <v>38</v>
       </c>
@@ -1727,7 +2021,7 @@
         <v>40790</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="5"/>
       <c r="B22" s="2" t="s">
         <v>40</v>
@@ -1742,7 +2036,7 @@
         <v>40796</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="B23" s="2" t="s">
         <v>19</v>
       </c>
@@ -1756,7 +2050,7 @@
         <v>40790</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="B24" s="2" t="s">
         <v>20</v>
       </c>
@@ -1770,7 +2064,7 @@
         <v>40790</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="B25" s="2" t="s">
         <v>30</v>
       </c>
@@ -1784,7 +2078,7 @@
         <v>40790</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="B26" s="2" t="s">
         <v>36</v>
       </c>
@@ -1798,7 +2092,7 @@
         <v>40790</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="B27" s="2" t="s">
         <v>40</v>
       </c>
@@ -1812,7 +2106,7 @@
         <v>40796</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="B28" s="2" t="s">
         <v>17</v>
       </c>
@@ -1826,7 +2120,7 @@
         <v>40804</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="B29" s="2" t="s">
         <v>31</v>
       </c>
@@ -1840,7 +2134,7 @@
         <v>40804</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="B30" s="2" t="s">
         <v>40</v>
       </c>
@@ -1854,7 +2148,7 @@
         <v>40810</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="B31" s="2" t="s">
         <v>26</v>
       </c>
@@ -1868,7 +2162,7 @@
         <v>40790</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" s="5"/>
       <c r="B32" s="2" t="s">
         <v>27</v>
@@ -1883,7 +2177,7 @@
         <v>40790</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5">
       <c r="B33" s="2" t="s">
         <v>28</v>
       </c>
@@ -1897,7 +2191,7 @@
         <v>40790</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:5">
       <c r="B34" s="2" t="s">
         <v>40</v>
       </c>
@@ -1911,7 +2205,7 @@
         <v>40796</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5">
       <c r="B35" s="2" t="s">
         <v>29</v>
       </c>
@@ -1925,7 +2219,7 @@
         <v>40804</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:5">
       <c r="B36" s="2" t="s">
         <v>40</v>
       </c>
@@ -1939,7 +2233,7 @@
         <v>40810</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:5">
       <c r="B37" s="2" t="s">
         <v>35</v>
       </c>
@@ -1953,7 +2247,7 @@
         <v>40790</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:5">
       <c r="B38" s="2" t="s">
         <v>40</v>
       </c>
@@ -1967,37 +2261,37 @@
         <v>40796</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:5">
       <c r="B39" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:5">
       <c r="B41" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:5">
       <c r="B42" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:5">
       <c r="B43" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:5">
       <c r="B44" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:5">
       <c r="B46" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:5">
       <c r="B47" s="2" t="s">
         <v>42</v>
       </c>
@@ -2011,7 +2305,7 @@
         <v>40810</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:5">
       <c r="B48" s="2" t="s">
         <v>40</v>
       </c>
@@ -2025,32 +2319,32 @@
         <v>40811</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:5">
       <c r="B49" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:5">
       <c r="B50" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:5">
       <c r="B51" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:5">
       <c r="C55" s="12" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:5">
       <c r="B57" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:5">
       <c r="B58" s="14" t="s">
         <v>64</v>
       </c>
@@ -2058,7 +2352,7 @@
       <c r="D58" s="8"/>
       <c r="E58" s="9"/>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:5">
       <c r="B59" s="14" t="s">
         <v>63</v>
       </c>
@@ -2066,7 +2360,7 @@
       <c r="D59" s="15"/>
       <c r="E59" s="9"/>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:5">
       <c r="B60" s="14" t="s">
         <v>62</v>
       </c>
@@ -2074,22 +2368,22 @@
       <c r="D60" s="11"/>
       <c r="E60" s="11"/>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:5">
       <c r="B61" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:5">
       <c r="B62" s="7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:5">
       <c r="B63" s="7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:5">
       <c r="B64" s="14" t="s">
         <v>61</v>
       </c>
@@ -2097,52 +2391,52 @@
       <c r="D64" s="10"/>
       <c r="E64" s="10"/>
     </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:10">
       <c r="B65" s="14" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:10">
       <c r="B66" s="13" t="s">
         <v>58</v>
       </c>
       <c r="F66" s="15"/>
       <c r="G66" s="15"/>
     </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:10">
       <c r="B67" s="13" t="s">
         <v>56</v>
       </c>
       <c r="H67" s="15"/>
       <c r="I67" s="15"/>
     </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:10">
       <c r="B68" s="13" t="s">
         <v>57</v>
       </c>
       <c r="H68" s="15"/>
       <c r="I68" s="15"/>
     </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:10">
       <c r="B69" s="13" t="s">
         <v>55</v>
       </c>
       <c r="I69" s="15"/>
       <c r="J69" s="15"/>
     </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:10">
       <c r="B70" s="13" t="s">
         <v>59</v>
       </c>
       <c r="I70" s="15"/>
       <c r="J70" s="15"/>
     </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:10">
       <c r="B72" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:10">
       <c r="B73" s="6" t="s">
         <v>55</v>
       </c>
@@ -2150,7 +2444,2625 @@
   </sheetData>
   <autoFilter ref="A1:E51"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N99"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="17" customFormat="1" ht="30">
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="N1" s="16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="18">
+        <v>40901</v>
+      </c>
+      <c r="I2" s="18">
+        <v>40901</v>
+      </c>
+      <c r="J2" t="s">
+        <v>84</v>
+      </c>
+      <c r="K2" s="18">
+        <v>40901</v>
+      </c>
+      <c r="L2" t="s">
+        <v>83</v>
+      </c>
+      <c r="M2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="B3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H3" s="18">
+        <v>40901</v>
+      </c>
+      <c r="I3" s="18">
+        <v>40902</v>
+      </c>
+      <c r="J3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="18">
+        <v>40901</v>
+      </c>
+      <c r="L3" t="s">
+        <v>87</v>
+      </c>
+      <c r="M3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="B4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H4" s="18">
+        <v>40901</v>
+      </c>
+      <c r="I4" s="18">
+        <v>40901</v>
+      </c>
+      <c r="J4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" s="18">
+        <v>40901</v>
+      </c>
+      <c r="L4" t="s">
+        <v>87</v>
+      </c>
+      <c r="M4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="B5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H5" s="18">
+        <v>40901</v>
+      </c>
+      <c r="I5" s="18">
+        <v>40902</v>
+      </c>
+      <c r="J5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5" s="18">
+        <v>40901</v>
+      </c>
+      <c r="L5" t="s">
+        <v>87</v>
+      </c>
+      <c r="M5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="B6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>87</v>
+      </c>
+      <c r="H6" s="18">
+        <v>40901</v>
+      </c>
+      <c r="I6" s="18">
+        <v>40901</v>
+      </c>
+      <c r="J6" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" s="18">
+        <v>40901</v>
+      </c>
+      <c r="L6" t="s">
+        <v>87</v>
+      </c>
+      <c r="M6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="B7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>87</v>
+      </c>
+      <c r="H7" s="18">
+        <v>40902</v>
+      </c>
+      <c r="I7" s="18">
+        <v>40902</v>
+      </c>
+      <c r="J7" t="s">
+        <v>39</v>
+      </c>
+      <c r="K7" s="18">
+        <v>40901</v>
+      </c>
+      <c r="L7" t="s">
+        <v>87</v>
+      </c>
+      <c r="M7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="B8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>87</v>
+      </c>
+      <c r="H8" s="18">
+        <v>40901</v>
+      </c>
+      <c r="I8" s="18">
+        <v>40901</v>
+      </c>
+      <c r="J8" t="s">
+        <v>39</v>
+      </c>
+      <c r="K8" s="18">
+        <v>40901</v>
+      </c>
+      <c r="L8" t="s">
+        <v>87</v>
+      </c>
+      <c r="M8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="B9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>87</v>
+      </c>
+      <c r="H9" s="18">
+        <v>40902</v>
+      </c>
+      <c r="I9" s="18">
+        <v>40902</v>
+      </c>
+      <c r="J9" t="s">
+        <v>39</v>
+      </c>
+      <c r="K9" s="18">
+        <v>40901</v>
+      </c>
+      <c r="L9" t="s">
+        <v>87</v>
+      </c>
+      <c r="M9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="B10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>87</v>
+      </c>
+      <c r="H10" s="18">
+        <v>40901</v>
+      </c>
+      <c r="I10" s="18">
+        <v>40902</v>
+      </c>
+      <c r="J10" t="s">
+        <v>9</v>
+      </c>
+      <c r="K10" s="18">
+        <v>40902</v>
+      </c>
+      <c r="L10" t="s">
+        <v>87</v>
+      </c>
+      <c r="M10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="B11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>87</v>
+      </c>
+      <c r="H11" s="18">
+        <v>40902</v>
+      </c>
+      <c r="I11" s="18">
+        <v>40902</v>
+      </c>
+      <c r="J11" t="s">
+        <v>9</v>
+      </c>
+      <c r="K11" s="18">
+        <v>40902</v>
+      </c>
+      <c r="L11" t="s">
+        <v>87</v>
+      </c>
+      <c r="M11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="B12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12" t="s">
+        <v>92</v>
+      </c>
+      <c r="E12" t="s">
+        <v>82</v>
+      </c>
+      <c r="G12" t="s">
+        <v>87</v>
+      </c>
+      <c r="H12" s="18">
+        <v>40901</v>
+      </c>
+      <c r="I12" s="18">
+        <v>40902</v>
+      </c>
+      <c r="J12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K12" s="18">
+        <v>40902</v>
+      </c>
+      <c r="L12" t="s">
+        <v>87</v>
+      </c>
+      <c r="M12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="B13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D13" t="s">
+        <v>92</v>
+      </c>
+      <c r="E13" t="s">
+        <v>82</v>
+      </c>
+      <c r="G13" t="s">
+        <v>87</v>
+      </c>
+      <c r="H13" s="18">
+        <v>40901</v>
+      </c>
+      <c r="I13" s="18">
+        <v>40902</v>
+      </c>
+      <c r="J13" t="s">
+        <v>6</v>
+      </c>
+      <c r="K13" s="18">
+        <v>40902</v>
+      </c>
+      <c r="L13" t="s">
+        <v>87</v>
+      </c>
+      <c r="M13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="B14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="18"/>
+      <c r="G14" t="s">
+        <v>87</v>
+      </c>
+      <c r="H14" s="18">
+        <v>40902</v>
+      </c>
+      <c r="I14" s="18">
+        <v>40903</v>
+      </c>
+      <c r="J14" t="s">
+        <v>6</v>
+      </c>
+      <c r="K14" s="18">
+        <v>40903</v>
+      </c>
+      <c r="L14" t="s">
+        <v>87</v>
+      </c>
+      <c r="M14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="B15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="D15" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" t="s">
+        <v>82</v>
+      </c>
+      <c r="F15" s="18"/>
+      <c r="G15" t="s">
+        <v>87</v>
+      </c>
+      <c r="H15" s="18">
+        <v>40901</v>
+      </c>
+      <c r="I15" s="18">
+        <v>40901</v>
+      </c>
+      <c r="J15" t="s">
+        <v>8</v>
+      </c>
+      <c r="K15" s="18">
+        <v>40902</v>
+      </c>
+      <c r="L15" t="s">
+        <v>87</v>
+      </c>
+      <c r="M15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="B16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16" t="s">
+        <v>103</v>
+      </c>
+      <c r="F16" s="18"/>
+      <c r="G16" t="s">
+        <v>87</v>
+      </c>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+    </row>
+    <row r="17" spans="2:11">
+      <c r="B17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" t="s">
+        <v>104</v>
+      </c>
+      <c r="D17" t="s">
+        <v>92</v>
+      </c>
+      <c r="E17" t="s">
+        <v>82</v>
+      </c>
+      <c r="F17">
+        <v>3</v>
+      </c>
+      <c r="G17" t="s">
+        <v>87</v>
+      </c>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" t="s">
+        <v>8</v>
+      </c>
+      <c r="K17" s="18"/>
+    </row>
+    <row r="18" spans="2:11">
+      <c r="B18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18" t="s">
+        <v>92</v>
+      </c>
+      <c r="E18" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18">
+        <v>4</v>
+      </c>
+      <c r="G18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11">
+      <c r="B19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" t="s">
+        <v>92</v>
+      </c>
+      <c r="E19" t="s">
+        <v>82</v>
+      </c>
+      <c r="F19">
+        <v>5</v>
+      </c>
+      <c r="G19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11">
+      <c r="B20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" t="s">
+        <v>107</v>
+      </c>
+      <c r="D20" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20" t="s">
+        <v>82</v>
+      </c>
+      <c r="F20">
+        <v>6</v>
+      </c>
+      <c r="G20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11">
+      <c r="B21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" t="s">
+        <v>108</v>
+      </c>
+      <c r="D21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F21">
+        <v>7</v>
+      </c>
+      <c r="G21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11">
+      <c r="B22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" t="s">
+        <v>92</v>
+      </c>
+      <c r="E22" t="s">
+        <v>82</v>
+      </c>
+      <c r="F22">
+        <v>8</v>
+      </c>
+      <c r="G22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11">
+      <c r="B23" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" t="s">
+        <v>92</v>
+      </c>
+      <c r="E23" t="s">
+        <v>82</v>
+      </c>
+      <c r="F23">
+        <v>9</v>
+      </c>
+      <c r="G23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11">
+      <c r="B24" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" t="s">
+        <v>109</v>
+      </c>
+      <c r="D24" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24" t="s">
+        <v>82</v>
+      </c>
+      <c r="F24">
+        <v>10</v>
+      </c>
+      <c r="G24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11">
+      <c r="B25" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" t="s">
+        <v>92</v>
+      </c>
+      <c r="E25" t="s">
+        <v>110</v>
+      </c>
+      <c r="F25">
+        <v>11</v>
+      </c>
+      <c r="G25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11">
+      <c r="B26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" t="s">
+        <v>92</v>
+      </c>
+      <c r="E26" t="s">
+        <v>110</v>
+      </c>
+      <c r="F26">
+        <v>12</v>
+      </c>
+      <c r="G26" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11">
+      <c r="B27" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" t="s">
+        <v>104</v>
+      </c>
+      <c r="D27" t="s">
+        <v>94</v>
+      </c>
+      <c r="E27" t="s">
+        <v>82</v>
+      </c>
+      <c r="F27">
+        <v>3</v>
+      </c>
+      <c r="G27" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11">
+      <c r="B28" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" t="s">
+        <v>105</v>
+      </c>
+      <c r="D28" t="s">
+        <v>94</v>
+      </c>
+      <c r="E28" t="s">
+        <v>82</v>
+      </c>
+      <c r="F28">
+        <v>4</v>
+      </c>
+      <c r="G28" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11">
+      <c r="B29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" t="s">
+        <v>106</v>
+      </c>
+      <c r="D29" t="s">
+        <v>94</v>
+      </c>
+      <c r="E29" t="s">
+        <v>82</v>
+      </c>
+      <c r="F29">
+        <v>5</v>
+      </c>
+      <c r="G29" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11">
+      <c r="B30" t="s">
+        <v>79</v>
+      </c>
+      <c r="C30" t="s">
+        <v>107</v>
+      </c>
+      <c r="D30" t="s">
+        <v>94</v>
+      </c>
+      <c r="E30" t="s">
+        <v>82</v>
+      </c>
+      <c r="F30">
+        <v>6</v>
+      </c>
+      <c r="G30" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11">
+      <c r="B31" t="s">
+        <v>79</v>
+      </c>
+      <c r="C31" t="s">
+        <v>108</v>
+      </c>
+      <c r="D31" t="s">
+        <v>94</v>
+      </c>
+      <c r="E31" t="s">
+        <v>82</v>
+      </c>
+      <c r="F31">
+        <v>7</v>
+      </c>
+      <c r="G31" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11">
+      <c r="B32" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" t="s">
+        <v>94</v>
+      </c>
+      <c r="E32" t="s">
+        <v>82</v>
+      </c>
+      <c r="F32">
+        <v>8</v>
+      </c>
+      <c r="G32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13">
+      <c r="B33" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" t="s">
+        <v>94</v>
+      </c>
+      <c r="E33" t="s">
+        <v>82</v>
+      </c>
+      <c r="F33">
+        <v>9</v>
+      </c>
+      <c r="G33" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13">
+      <c r="B34" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34" t="s">
+        <v>109</v>
+      </c>
+      <c r="D34" t="s">
+        <v>94</v>
+      </c>
+      <c r="E34" t="s">
+        <v>82</v>
+      </c>
+      <c r="F34">
+        <v>10</v>
+      </c>
+      <c r="G34" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13">
+      <c r="B35" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" t="s">
+        <v>94</v>
+      </c>
+      <c r="E35" t="s">
+        <v>110</v>
+      </c>
+      <c r="F35">
+        <v>11</v>
+      </c>
+      <c r="G35" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13">
+      <c r="B36" t="s">
+        <v>79</v>
+      </c>
+      <c r="C36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" t="s">
+        <v>94</v>
+      </c>
+      <c r="E36" t="s">
+        <v>110</v>
+      </c>
+      <c r="F36">
+        <v>12</v>
+      </c>
+      <c r="G36" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13">
+      <c r="B37" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" t="s">
+        <v>104</v>
+      </c>
+      <c r="D37" t="s">
+        <v>44</v>
+      </c>
+      <c r="E37" t="s">
+        <v>82</v>
+      </c>
+      <c r="F37">
+        <v>3</v>
+      </c>
+      <c r="G37" t="s">
+        <v>87</v>
+      </c>
+      <c r="J37" t="s">
+        <v>9</v>
+      </c>
+      <c r="K37" s="18"/>
+      <c r="L37" t="s">
+        <v>87</v>
+      </c>
+      <c r="M37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13">
+      <c r="B38" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" t="s">
+        <v>105</v>
+      </c>
+      <c r="D38" t="s">
+        <v>44</v>
+      </c>
+      <c r="E38" t="s">
+        <v>82</v>
+      </c>
+      <c r="F38">
+        <v>4</v>
+      </c>
+      <c r="G38" t="s">
+        <v>87</v>
+      </c>
+      <c r="J38" t="s">
+        <v>9</v>
+      </c>
+      <c r="K38" s="18"/>
+      <c r="L38" t="s">
+        <v>87</v>
+      </c>
+      <c r="M38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="2:13">
+      <c r="B39" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39" t="s">
+        <v>106</v>
+      </c>
+      <c r="D39" t="s">
+        <v>44</v>
+      </c>
+      <c r="E39" t="s">
+        <v>82</v>
+      </c>
+      <c r="F39">
+        <v>5</v>
+      </c>
+      <c r="G39" t="s">
+        <v>87</v>
+      </c>
+      <c r="J39" t="s">
+        <v>9</v>
+      </c>
+      <c r="L39" t="s">
+        <v>87</v>
+      </c>
+      <c r="M39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="2:13">
+      <c r="B40" t="s">
+        <v>79</v>
+      </c>
+      <c r="C40" t="s">
+        <v>107</v>
+      </c>
+      <c r="D40" t="s">
+        <v>44</v>
+      </c>
+      <c r="E40" t="s">
+        <v>82</v>
+      </c>
+      <c r="F40">
+        <v>6</v>
+      </c>
+      <c r="G40" t="s">
+        <v>87</v>
+      </c>
+      <c r="J40" t="s">
+        <v>9</v>
+      </c>
+      <c r="L40" t="s">
+        <v>87</v>
+      </c>
+      <c r="M40" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="2:13">
+      <c r="B41" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" t="s">
+        <v>108</v>
+      </c>
+      <c r="D41" t="s">
+        <v>44</v>
+      </c>
+      <c r="E41" t="s">
+        <v>82</v>
+      </c>
+      <c r="F41">
+        <v>7</v>
+      </c>
+      <c r="G41" t="s">
+        <v>87</v>
+      </c>
+      <c r="J41" t="s">
+        <v>9</v>
+      </c>
+      <c r="L41" t="s">
+        <v>87</v>
+      </c>
+      <c r="M41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="2:13">
+      <c r="B42" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42" t="s">
+        <v>30</v>
+      </c>
+      <c r="D42" t="s">
+        <v>44</v>
+      </c>
+      <c r="E42" t="s">
+        <v>82</v>
+      </c>
+      <c r="F42">
+        <v>8</v>
+      </c>
+      <c r="G42" t="s">
+        <v>87</v>
+      </c>
+      <c r="J42" t="s">
+        <v>9</v>
+      </c>
+      <c r="L42" t="s">
+        <v>87</v>
+      </c>
+      <c r="M42" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="2:13">
+      <c r="B43" t="s">
+        <v>79</v>
+      </c>
+      <c r="C43" t="s">
+        <v>12</v>
+      </c>
+      <c r="D43" t="s">
+        <v>44</v>
+      </c>
+      <c r="E43" t="s">
+        <v>82</v>
+      </c>
+      <c r="F43">
+        <v>9</v>
+      </c>
+      <c r="G43" t="s">
+        <v>87</v>
+      </c>
+      <c r="J43" t="s">
+        <v>9</v>
+      </c>
+      <c r="L43" t="s">
+        <v>87</v>
+      </c>
+      <c r="M43" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="2:13">
+      <c r="B44" t="s">
+        <v>79</v>
+      </c>
+      <c r="C44" t="s">
+        <v>109</v>
+      </c>
+      <c r="D44" t="s">
+        <v>44</v>
+      </c>
+      <c r="E44" t="s">
+        <v>82</v>
+      </c>
+      <c r="F44">
+        <v>10</v>
+      </c>
+      <c r="G44" t="s">
+        <v>87</v>
+      </c>
+      <c r="J44" t="s">
+        <v>9</v>
+      </c>
+      <c r="L44" t="s">
+        <v>87</v>
+      </c>
+      <c r="M44" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="2:13">
+      <c r="B45" t="s">
+        <v>79</v>
+      </c>
+      <c r="C45" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45" t="s">
+        <v>44</v>
+      </c>
+      <c r="E45" t="s">
+        <v>110</v>
+      </c>
+      <c r="F45">
+        <v>11</v>
+      </c>
+      <c r="G45" t="s">
+        <v>87</v>
+      </c>
+      <c r="J45" t="s">
+        <v>9</v>
+      </c>
+      <c r="L45" t="s">
+        <v>87</v>
+      </c>
+      <c r="M45" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="2:13">
+      <c r="B46" t="s">
+        <v>79</v>
+      </c>
+      <c r="C46" t="s">
+        <v>22</v>
+      </c>
+      <c r="D46" t="s">
+        <v>44</v>
+      </c>
+      <c r="E46" t="s">
+        <v>110</v>
+      </c>
+      <c r="F46">
+        <v>12</v>
+      </c>
+      <c r="G46" t="s">
+        <v>87</v>
+      </c>
+      <c r="J46" t="s">
+        <v>9</v>
+      </c>
+      <c r="L46" t="s">
+        <v>87</v>
+      </c>
+      <c r="M46" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="2:13">
+      <c r="B47" t="s">
+        <v>111</v>
+      </c>
+      <c r="C47" t="s">
+        <v>112</v>
+      </c>
+      <c r="D47" t="s">
+        <v>92</v>
+      </c>
+      <c r="E47" t="s">
+        <v>82</v>
+      </c>
+      <c r="F47">
+        <v>1</v>
+      </c>
+      <c r="G47" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="2:13">
+      <c r="B48" t="s">
+        <v>111</v>
+      </c>
+      <c r="C48" t="s">
+        <v>113</v>
+      </c>
+      <c r="D48" t="s">
+        <v>92</v>
+      </c>
+      <c r="E48" t="s">
+        <v>82</v>
+      </c>
+      <c r="F48">
+        <v>2</v>
+      </c>
+      <c r="G48" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="2:13">
+      <c r="B49" t="s">
+        <v>111</v>
+      </c>
+      <c r="C49" t="s">
+        <v>114</v>
+      </c>
+      <c r="D49" t="s">
+        <v>92</v>
+      </c>
+      <c r="E49" t="s">
+        <v>82</v>
+      </c>
+      <c r="F49">
+        <v>3</v>
+      </c>
+      <c r="G49" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="50" spans="2:13">
+      <c r="B50" t="s">
+        <v>111</v>
+      </c>
+      <c r="C50" t="s">
+        <v>115</v>
+      </c>
+      <c r="D50" t="s">
+        <v>92</v>
+      </c>
+      <c r="E50" t="s">
+        <v>82</v>
+      </c>
+      <c r="F50">
+        <v>4</v>
+      </c>
+      <c r="G50" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="51" spans="2:13">
+      <c r="B51" t="s">
+        <v>111</v>
+      </c>
+      <c r="C51" t="s">
+        <v>106</v>
+      </c>
+      <c r="D51" t="s">
+        <v>92</v>
+      </c>
+      <c r="E51" t="s">
+        <v>82</v>
+      </c>
+      <c r="F51">
+        <v>5</v>
+      </c>
+      <c r="G51" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="52" spans="2:13">
+      <c r="B52" t="s">
+        <v>111</v>
+      </c>
+      <c r="C52" t="s">
+        <v>18</v>
+      </c>
+      <c r="D52" t="s">
+        <v>92</v>
+      </c>
+      <c r="E52" t="s">
+        <v>103</v>
+      </c>
+      <c r="F52">
+        <v>6</v>
+      </c>
+      <c r="G52" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="53" spans="2:13">
+      <c r="B53" t="s">
+        <v>111</v>
+      </c>
+      <c r="C53" t="s">
+        <v>116</v>
+      </c>
+      <c r="D53" t="s">
+        <v>92</v>
+      </c>
+      <c r="E53" t="s">
+        <v>103</v>
+      </c>
+      <c r="F53">
+        <v>7</v>
+      </c>
+      <c r="G53" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="54" spans="2:13">
+      <c r="B54" t="s">
+        <v>111</v>
+      </c>
+      <c r="C54" t="s">
+        <v>117</v>
+      </c>
+      <c r="D54" t="s">
+        <v>92</v>
+      </c>
+      <c r="E54" t="s">
+        <v>103</v>
+      </c>
+      <c r="F54">
+        <v>8</v>
+      </c>
+      <c r="G54" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="55" spans="2:13">
+      <c r="B55" t="s">
+        <v>111</v>
+      </c>
+      <c r="C55" t="s">
+        <v>112</v>
+      </c>
+      <c r="D55" t="s">
+        <v>94</v>
+      </c>
+      <c r="E55" t="s">
+        <v>82</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="G55" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="56" spans="2:13">
+      <c r="B56" t="s">
+        <v>111</v>
+      </c>
+      <c r="C56" t="s">
+        <v>113</v>
+      </c>
+      <c r="D56" t="s">
+        <v>94</v>
+      </c>
+      <c r="E56" t="s">
+        <v>82</v>
+      </c>
+      <c r="F56">
+        <v>2</v>
+      </c>
+      <c r="G56" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="57" spans="2:13">
+      <c r="B57" t="s">
+        <v>111</v>
+      </c>
+      <c r="C57" t="s">
+        <v>114</v>
+      </c>
+      <c r="D57" t="s">
+        <v>94</v>
+      </c>
+      <c r="E57" t="s">
+        <v>82</v>
+      </c>
+      <c r="F57">
+        <v>3</v>
+      </c>
+      <c r="G57" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="58" spans="2:13">
+      <c r="B58" t="s">
+        <v>111</v>
+      </c>
+      <c r="C58" t="s">
+        <v>115</v>
+      </c>
+      <c r="D58" t="s">
+        <v>94</v>
+      </c>
+      <c r="E58" t="s">
+        <v>82</v>
+      </c>
+      <c r="F58">
+        <v>4</v>
+      </c>
+      <c r="G58" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="59" spans="2:13">
+      <c r="B59" t="s">
+        <v>111</v>
+      </c>
+      <c r="C59" t="s">
+        <v>106</v>
+      </c>
+      <c r="D59" t="s">
+        <v>94</v>
+      </c>
+      <c r="E59" t="s">
+        <v>82</v>
+      </c>
+      <c r="F59">
+        <v>5</v>
+      </c>
+      <c r="G59" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="60" spans="2:13">
+      <c r="B60" t="s">
+        <v>111</v>
+      </c>
+      <c r="C60" t="s">
+        <v>18</v>
+      </c>
+      <c r="D60" t="s">
+        <v>94</v>
+      </c>
+      <c r="E60" t="s">
+        <v>103</v>
+      </c>
+      <c r="F60">
+        <v>6</v>
+      </c>
+      <c r="G60" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="61" spans="2:13">
+      <c r="B61" t="s">
+        <v>111</v>
+      </c>
+      <c r="C61" t="s">
+        <v>116</v>
+      </c>
+      <c r="D61" t="s">
+        <v>94</v>
+      </c>
+      <c r="E61" t="s">
+        <v>103</v>
+      </c>
+      <c r="F61">
+        <v>7</v>
+      </c>
+      <c r="G61" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="62" spans="2:13">
+      <c r="B62" t="s">
+        <v>111</v>
+      </c>
+      <c r="C62" t="s">
+        <v>117</v>
+      </c>
+      <c r="D62" t="s">
+        <v>94</v>
+      </c>
+      <c r="E62" t="s">
+        <v>103</v>
+      </c>
+      <c r="F62">
+        <v>8</v>
+      </c>
+      <c r="G62" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="63" spans="2:13">
+      <c r="B63" t="s">
+        <v>111</v>
+      </c>
+      <c r="C63" t="s">
+        <v>112</v>
+      </c>
+      <c r="D63" t="s">
+        <v>44</v>
+      </c>
+      <c r="E63" t="s">
+        <v>82</v>
+      </c>
+      <c r="F63">
+        <v>1</v>
+      </c>
+      <c r="G63" t="s">
+        <v>87</v>
+      </c>
+      <c r="J63" t="s">
+        <v>9</v>
+      </c>
+      <c r="K63" s="18"/>
+      <c r="L63" t="s">
+        <v>87</v>
+      </c>
+      <c r="M63" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="2:13">
+      <c r="B64" t="s">
+        <v>111</v>
+      </c>
+      <c r="C64" t="s">
+        <v>113</v>
+      </c>
+      <c r="D64" t="s">
+        <v>44</v>
+      </c>
+      <c r="E64" t="s">
+        <v>82</v>
+      </c>
+      <c r="F64">
+        <v>2</v>
+      </c>
+      <c r="G64" t="s">
+        <v>87</v>
+      </c>
+      <c r="J64" t="s">
+        <v>9</v>
+      </c>
+      <c r="K64" s="18"/>
+      <c r="L64" t="s">
+        <v>87</v>
+      </c>
+      <c r="M64" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="2:13">
+      <c r="B65" t="s">
+        <v>111</v>
+      </c>
+      <c r="C65" t="s">
+        <v>114</v>
+      </c>
+      <c r="D65" t="s">
+        <v>44</v>
+      </c>
+      <c r="E65" t="s">
+        <v>82</v>
+      </c>
+      <c r="F65">
+        <v>3</v>
+      </c>
+      <c r="G65" t="s">
+        <v>87</v>
+      </c>
+      <c r="J65" t="s">
+        <v>9</v>
+      </c>
+      <c r="L65" t="s">
+        <v>87</v>
+      </c>
+      <c r="M65" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="2:13">
+      <c r="B66" t="s">
+        <v>111</v>
+      </c>
+      <c r="C66" t="s">
+        <v>115</v>
+      </c>
+      <c r="D66" t="s">
+        <v>44</v>
+      </c>
+      <c r="E66" t="s">
+        <v>82</v>
+      </c>
+      <c r="F66">
+        <v>4</v>
+      </c>
+      <c r="G66" t="s">
+        <v>87</v>
+      </c>
+      <c r="J66" t="s">
+        <v>9</v>
+      </c>
+      <c r="L66" t="s">
+        <v>87</v>
+      </c>
+      <c r="M66" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="2:13">
+      <c r="B67" t="s">
+        <v>111</v>
+      </c>
+      <c r="C67" t="s">
+        <v>106</v>
+      </c>
+      <c r="D67" t="s">
+        <v>44</v>
+      </c>
+      <c r="E67" t="s">
+        <v>82</v>
+      </c>
+      <c r="F67">
+        <v>5</v>
+      </c>
+      <c r="G67" t="s">
+        <v>87</v>
+      </c>
+      <c r="J67" t="s">
+        <v>9</v>
+      </c>
+      <c r="L67" t="s">
+        <v>87</v>
+      </c>
+      <c r="M67" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="2:13">
+      <c r="B68" t="s">
+        <v>111</v>
+      </c>
+      <c r="C68" t="s">
+        <v>18</v>
+      </c>
+      <c r="D68" t="s">
+        <v>44</v>
+      </c>
+      <c r="E68" t="s">
+        <v>103</v>
+      </c>
+      <c r="F68">
+        <v>6</v>
+      </c>
+      <c r="G68" t="s">
+        <v>87</v>
+      </c>
+      <c r="J68" t="s">
+        <v>9</v>
+      </c>
+      <c r="L68" t="s">
+        <v>87</v>
+      </c>
+      <c r="M68" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="2:13">
+      <c r="B69" t="s">
+        <v>111</v>
+      </c>
+      <c r="C69" t="s">
+        <v>116</v>
+      </c>
+      <c r="D69" t="s">
+        <v>44</v>
+      </c>
+      <c r="E69" t="s">
+        <v>103</v>
+      </c>
+      <c r="F69">
+        <v>7</v>
+      </c>
+      <c r="G69" t="s">
+        <v>87</v>
+      </c>
+      <c r="J69" t="s">
+        <v>9</v>
+      </c>
+      <c r="L69" t="s">
+        <v>87</v>
+      </c>
+      <c r="M69" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="2:13">
+      <c r="B70" t="s">
+        <v>111</v>
+      </c>
+      <c r="C70" t="s">
+        <v>117</v>
+      </c>
+      <c r="D70" t="s">
+        <v>44</v>
+      </c>
+      <c r="E70" t="s">
+        <v>103</v>
+      </c>
+      <c r="F70">
+        <v>8</v>
+      </c>
+      <c r="G70" t="s">
+        <v>87</v>
+      </c>
+      <c r="J70" t="s">
+        <v>9</v>
+      </c>
+      <c r="L70" t="s">
+        <v>87</v>
+      </c>
+      <c r="M70" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="2:13">
+      <c r="B71" t="s">
+        <v>118</v>
+      </c>
+      <c r="C71" t="s">
+        <v>119</v>
+      </c>
+      <c r="D71" t="s">
+        <v>92</v>
+      </c>
+      <c r="E71" t="s">
+        <v>82</v>
+      </c>
+      <c r="F71">
+        <v>1</v>
+      </c>
+      <c r="G71" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="72" spans="2:13">
+      <c r="B72" t="s">
+        <v>118</v>
+      </c>
+      <c r="C72" t="s">
+        <v>120</v>
+      </c>
+      <c r="D72" t="s">
+        <v>92</v>
+      </c>
+      <c r="E72" t="s">
+        <v>82</v>
+      </c>
+      <c r="F72">
+        <v>2</v>
+      </c>
+      <c r="G72" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="73" spans="2:13">
+      <c r="B73" t="s">
+        <v>118</v>
+      </c>
+      <c r="C73" t="s">
+        <v>121</v>
+      </c>
+      <c r="D73" t="s">
+        <v>92</v>
+      </c>
+      <c r="E73" t="s">
+        <v>82</v>
+      </c>
+      <c r="F73">
+        <v>3</v>
+      </c>
+      <c r="G73" s="19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="74" spans="2:13">
+      <c r="C74" t="s">
+        <v>119</v>
+      </c>
+      <c r="D74" t="s">
+        <v>94</v>
+      </c>
+      <c r="E74" t="s">
+        <v>82</v>
+      </c>
+      <c r="F74">
+        <v>1</v>
+      </c>
+      <c r="G74" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="75" spans="2:13">
+      <c r="C75" t="s">
+        <v>120</v>
+      </c>
+      <c r="D75" t="s">
+        <v>94</v>
+      </c>
+      <c r="E75" t="s">
+        <v>82</v>
+      </c>
+      <c r="F75">
+        <v>2</v>
+      </c>
+      <c r="G75" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="76" spans="2:13">
+      <c r="C76" t="s">
+        <v>121</v>
+      </c>
+      <c r="D76" t="s">
+        <v>94</v>
+      </c>
+      <c r="E76" t="s">
+        <v>82</v>
+      </c>
+      <c r="F76">
+        <v>3</v>
+      </c>
+      <c r="G76" s="19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="77" spans="2:13">
+      <c r="C77" t="s">
+        <v>119</v>
+      </c>
+      <c r="D77" t="s">
+        <v>44</v>
+      </c>
+      <c r="E77" t="s">
+        <v>82</v>
+      </c>
+      <c r="F77">
+        <v>1</v>
+      </c>
+      <c r="G77" t="s">
+        <v>87</v>
+      </c>
+      <c r="J77" t="s">
+        <v>9</v>
+      </c>
+      <c r="K77" s="18"/>
+      <c r="L77" t="s">
+        <v>87</v>
+      </c>
+      <c r="M77" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="2:13">
+      <c r="C78" t="s">
+        <v>120</v>
+      </c>
+      <c r="D78" t="s">
+        <v>44</v>
+      </c>
+      <c r="E78" t="s">
+        <v>82</v>
+      </c>
+      <c r="F78">
+        <v>2</v>
+      </c>
+      <c r="G78" t="s">
+        <v>87</v>
+      </c>
+      <c r="J78" t="s">
+        <v>9</v>
+      </c>
+      <c r="K78" s="18"/>
+      <c r="L78" t="s">
+        <v>87</v>
+      </c>
+      <c r="M78" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79" spans="2:13">
+      <c r="C79" t="s">
+        <v>121</v>
+      </c>
+      <c r="D79" t="s">
+        <v>44</v>
+      </c>
+      <c r="E79" t="s">
+        <v>82</v>
+      </c>
+      <c r="F79">
+        <v>3</v>
+      </c>
+      <c r="G79" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="J79" t="s">
+        <v>9</v>
+      </c>
+      <c r="L79" t="s">
+        <v>87</v>
+      </c>
+      <c r="M79" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" spans="2:13">
+      <c r="B80" t="s">
+        <v>101</v>
+      </c>
+      <c r="C80" t="s">
+        <v>122</v>
+      </c>
+      <c r="D80" t="s">
+        <v>92</v>
+      </c>
+      <c r="E80" t="s">
+        <v>82</v>
+      </c>
+      <c r="F80">
+        <v>1</v>
+      </c>
+      <c r="G80" s="19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="81" spans="2:13">
+      <c r="B81" t="s">
+        <v>123</v>
+      </c>
+      <c r="C81" t="s">
+        <v>124</v>
+      </c>
+      <c r="D81" t="s">
+        <v>92</v>
+      </c>
+      <c r="E81" t="s">
+        <v>110</v>
+      </c>
+      <c r="F81">
+        <v>1</v>
+      </c>
+      <c r="G81" s="19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="82" spans="2:13">
+      <c r="B82" t="s">
+        <v>123</v>
+      </c>
+      <c r="C82" t="s">
+        <v>32</v>
+      </c>
+      <c r="D82" t="s">
+        <v>92</v>
+      </c>
+      <c r="E82" t="s">
+        <v>110</v>
+      </c>
+      <c r="F82">
+        <v>2</v>
+      </c>
+      <c r="G82" s="19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="83" spans="2:13">
+      <c r="B83" t="s">
+        <v>125</v>
+      </c>
+      <c r="C83" t="s">
+        <v>126</v>
+      </c>
+      <c r="D83" t="s">
+        <v>92</v>
+      </c>
+      <c r="E83" t="s">
+        <v>110</v>
+      </c>
+      <c r="F83">
+        <v>1</v>
+      </c>
+      <c r="G83" s="19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="84" spans="2:13">
+      <c r="B84" t="s">
+        <v>125</v>
+      </c>
+      <c r="C84" t="s">
+        <v>127</v>
+      </c>
+      <c r="D84" t="s">
+        <v>92</v>
+      </c>
+      <c r="E84" t="s">
+        <v>110</v>
+      </c>
+      <c r="F84">
+        <v>2</v>
+      </c>
+      <c r="G84" s="19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="85" spans="2:13">
+      <c r="B85" t="s">
+        <v>125</v>
+      </c>
+      <c r="C85" t="s">
+        <v>128</v>
+      </c>
+      <c r="D85" t="s">
+        <v>92</v>
+      </c>
+      <c r="E85" t="s">
+        <v>110</v>
+      </c>
+      <c r="F85">
+        <v>3</v>
+      </c>
+      <c r="G85" s="19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="86" spans="2:13">
+      <c r="B86" t="s">
+        <v>125</v>
+      </c>
+      <c r="C86" t="s">
+        <v>23</v>
+      </c>
+      <c r="D86" t="s">
+        <v>92</v>
+      </c>
+      <c r="E86" t="s">
+        <v>110</v>
+      </c>
+      <c r="F86">
+        <v>4</v>
+      </c>
+      <c r="G86" s="19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="87" spans="2:13">
+      <c r="B87" t="s">
+        <v>125</v>
+      </c>
+      <c r="C87" t="s">
+        <v>22</v>
+      </c>
+      <c r="D87" t="s">
+        <v>92</v>
+      </c>
+      <c r="E87" t="s">
+        <v>110</v>
+      </c>
+      <c r="F87">
+        <v>1</v>
+      </c>
+      <c r="G87" s="19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="88" spans="2:13">
+      <c r="B88" t="s">
+        <v>81</v>
+      </c>
+      <c r="C88" t="s">
+        <v>129</v>
+      </c>
+      <c r="D88" t="s">
+        <v>81</v>
+      </c>
+      <c r="E88" t="s">
+        <v>82</v>
+      </c>
+      <c r="F88">
+        <v>1</v>
+      </c>
+      <c r="G88" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="H88" s="18">
+        <v>40901</v>
+      </c>
+      <c r="I88" s="18">
+        <v>40901</v>
+      </c>
+      <c r="J88" t="s">
+        <v>39</v>
+      </c>
+      <c r="K88" s="18">
+        <v>40901</v>
+      </c>
+      <c r="L88" t="s">
+        <v>87</v>
+      </c>
+      <c r="M88" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="89" spans="2:13">
+      <c r="B89" t="s">
+        <v>130</v>
+      </c>
+      <c r="C89" t="s">
+        <v>131</v>
+      </c>
+      <c r="D89" t="s">
+        <v>130</v>
+      </c>
+      <c r="E89" t="s">
+        <v>82</v>
+      </c>
+      <c r="F89">
+        <v>2</v>
+      </c>
+      <c r="G89" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="J89" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90" spans="2:13">
+      <c r="B90" t="s">
+        <v>130</v>
+      </c>
+      <c r="C90" t="s">
+        <v>132</v>
+      </c>
+      <c r="D90" t="s">
+        <v>130</v>
+      </c>
+      <c r="E90" t="s">
+        <v>103</v>
+      </c>
+      <c r="F90">
+        <v>6</v>
+      </c>
+      <c r="G90" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="J90" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="91" spans="2:13">
+      <c r="B91" t="s">
+        <v>130</v>
+      </c>
+      <c r="C91" t="s">
+        <v>133</v>
+      </c>
+      <c r="D91" t="s">
+        <v>130</v>
+      </c>
+      <c r="E91" t="s">
+        <v>103</v>
+      </c>
+      <c r="F91">
+        <v>7</v>
+      </c>
+      <c r="G91" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="J91" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="92" spans="2:13">
+      <c r="B92" t="s">
+        <v>130</v>
+      </c>
+      <c r="C92" t="s">
+        <v>134</v>
+      </c>
+      <c r="D92" t="s">
+        <v>130</v>
+      </c>
+      <c r="E92" t="s">
+        <v>82</v>
+      </c>
+      <c r="F92">
+        <v>4</v>
+      </c>
+      <c r="G92" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="H92" s="18">
+        <v>40901</v>
+      </c>
+      <c r="J92" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="93" spans="2:13">
+      <c r="B93" t="s">
+        <v>130</v>
+      </c>
+      <c r="C93" t="s">
+        <v>136</v>
+      </c>
+      <c r="D93" t="s">
+        <v>130</v>
+      </c>
+      <c r="E93" t="s">
+        <v>82</v>
+      </c>
+      <c r="F93">
+        <v>5</v>
+      </c>
+      <c r="G93" s="19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="94" spans="2:13">
+      <c r="B94" t="s">
+        <v>130</v>
+      </c>
+      <c r="C94" t="s">
+        <v>137</v>
+      </c>
+      <c r="D94" t="s">
+        <v>130</v>
+      </c>
+      <c r="E94" t="s">
+        <v>82</v>
+      </c>
+      <c r="F94">
+        <v>3</v>
+      </c>
+      <c r="G94" s="19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="95" spans="2:13">
+      <c r="B95" t="s">
+        <v>130</v>
+      </c>
+      <c r="C95" t="s">
+        <v>138</v>
+      </c>
+      <c r="D95" t="s">
+        <v>130</v>
+      </c>
+      <c r="E95" t="s">
+        <v>82</v>
+      </c>
+      <c r="F95">
+        <v>1</v>
+      </c>
+      <c r="G95" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="J95" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="96" spans="2:13">
+      <c r="B96" t="s">
+        <v>123</v>
+      </c>
+      <c r="C96" t="s">
+        <v>139</v>
+      </c>
+      <c r="D96" t="s">
+        <v>92</v>
+      </c>
+      <c r="E96" t="s">
+        <v>82</v>
+      </c>
+      <c r="F96">
+        <v>1</v>
+      </c>
+      <c r="G96" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="H96" s="18">
+        <v>40901</v>
+      </c>
+      <c r="I96" s="18">
+        <v>40901</v>
+      </c>
+      <c r="J96" t="s">
+        <v>8</v>
+      </c>
+      <c r="K96" s="18">
+        <v>40902</v>
+      </c>
+      <c r="L96" t="s">
+        <v>87</v>
+      </c>
+      <c r="M96" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="97" spans="2:10">
+      <c r="B97" t="s">
+        <v>101</v>
+      </c>
+      <c r="C97" t="s">
+        <v>140</v>
+      </c>
+      <c r="D97" t="s">
+        <v>92</v>
+      </c>
+      <c r="E97" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="98" spans="2:10">
+      <c r="B98" t="s">
+        <v>101</v>
+      </c>
+      <c r="C98" t="s">
+        <v>141</v>
+      </c>
+      <c r="D98" t="s">
+        <v>92</v>
+      </c>
+      <c r="E98" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="99" spans="2:10">
+      <c r="B99" t="s">
+        <v>101</v>
+      </c>
+      <c r="C99" t="s">
+        <v>142</v>
+      </c>
+      <c r="D99" t="s">
+        <v>92</v>
+      </c>
+      <c r="E99" t="s">
+        <v>110</v>
+      </c>
+      <c r="F99">
+        <v>1</v>
+      </c>
+      <c r="G99" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="J99" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:N99"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Updated Misc Tasks yet to assign tab and Tasks statues
</commit_message>
<xml_diff>
--- a/docs/PM-1 Project Management/PM-1.2 Plans/PM-1.2.1 Project Plan/vms_implementation_plan_v0.1a.xlsx
+++ b/docs/PM-1 Project Management/PM-1.2 Plans/PM-1.2.1 Project Plan/vms_implementation_plan_v0.1a.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14320" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="25600" windowHeight="14320" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$51</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tasks!$A$1:$N$99</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tasks!$A$1:$N$100</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="154">
   <si>
     <t>No</t>
   </si>
@@ -639,6 +639,27 @@
   </si>
   <si>
     <t>Audit Log Meeting Minutes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Validator</t>
+  </si>
+  <si>
+    <t>Utility Classes</t>
+  </si>
+  <si>
+    <t>Use of messages.properties</t>
+  </si>
+  <si>
+    <t>How to use DWR</t>
+  </si>
+  <si>
+    <t>Upgrade Jasper Lib</t>
+  </si>
+  <si>
+    <t>Database Script</t>
   </si>
 </sst>
 </file>
@@ -802,8 +823,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="267">
+  <cellStyleXfs count="287">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1106,7 +1147,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="267">
+  <cellStyles count="287">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1240,6 +1281,16 @@
     <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1373,6 +1424,16 @@
     <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2455,10 +2516,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N99"/>
+  <dimension ref="A1:N100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2571,7 +2632,7 @@
         <v>82</v>
       </c>
       <c r="G3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H3" s="18">
         <v>40901</v>
@@ -2586,7 +2647,7 @@
         <v>40901</v>
       </c>
       <c r="L3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="M3" t="s">
         <v>6</v>
@@ -2606,7 +2667,7 @@
         <v>82</v>
       </c>
       <c r="G4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H4" s="18">
         <v>40901</v>
@@ -2624,33 +2685,36 @@
         <v>87</v>
       </c>
       <c r="M4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="B5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C5" t="s">
-        <v>89</v>
+        <v>129</v>
       </c>
       <c r="D5" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="E5" t="s">
         <v>82</v>
       </c>
-      <c r="G5" t="s">
-        <v>87</v>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>83</v>
       </c>
       <c r="H5" s="18">
         <v>40901</v>
       </c>
       <c r="I5" s="18">
-        <v>40902</v>
+        <v>40901</v>
       </c>
       <c r="J5" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="K5" s="18">
         <v>40901</v>
@@ -2659,7 +2723,7 @@
         <v>87</v>
       </c>
       <c r="M5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -2667,28 +2731,25 @@
         <v>79</v>
       </c>
       <c r="C6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E6" t="s">
         <v>82</v>
       </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
       <c r="G6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H6" s="18">
         <v>40901</v>
       </c>
       <c r="I6" s="18">
-        <v>40901</v>
+        <v>40902</v>
       </c>
       <c r="J6" t="s">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="K6" s="18">
         <v>40901</v>
@@ -2705,7 +2766,7 @@
         <v>79</v>
       </c>
       <c r="C7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D7" t="s">
         <v>92</v>
@@ -2714,16 +2775,16 @@
         <v>82</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7" t="s">
         <v>87</v>
       </c>
       <c r="H7" s="18">
-        <v>40902</v>
+        <v>40901</v>
       </c>
       <c r="I7" s="18">
-        <v>40902</v>
+        <v>40901</v>
       </c>
       <c r="J7" t="s">
         <v>39</v>
@@ -2743,25 +2804,25 @@
         <v>79</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E8" t="s">
         <v>82</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8" t="s">
         <v>87</v>
       </c>
       <c r="H8" s="18">
-        <v>40901</v>
+        <v>40902</v>
       </c>
       <c r="I8" s="18">
-        <v>40901</v>
+        <v>40902</v>
       </c>
       <c r="J8" t="s">
         <v>39</v>
@@ -2781,7 +2842,7 @@
         <v>79</v>
       </c>
       <c r="C9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D9" t="s">
         <v>94</v>
@@ -2790,16 +2851,16 @@
         <v>82</v>
       </c>
       <c r="F9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9" t="s">
         <v>87</v>
       </c>
       <c r="H9" s="18">
-        <v>40902</v>
+        <v>40901</v>
       </c>
       <c r="I9" s="18">
-        <v>40902</v>
+        <v>40901</v>
       </c>
       <c r="J9" t="s">
         <v>39</v>
@@ -2819,31 +2880,31 @@
         <v>79</v>
       </c>
       <c r="C10" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D10" t="s">
-        <v>44</v>
+        <v>94</v>
       </c>
       <c r="E10" t="s">
         <v>82</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G10" t="s">
         <v>87</v>
       </c>
       <c r="H10" s="18">
-        <v>40901</v>
+        <v>40902</v>
       </c>
       <c r="I10" s="18">
         <v>40902</v>
       </c>
       <c r="J10" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="K10" s="18">
-        <v>40902</v>
+        <v>40901</v>
       </c>
       <c r="L10" t="s">
         <v>87</v>
@@ -2857,7 +2918,7 @@
         <v>79</v>
       </c>
       <c r="C11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D11" t="s">
         <v>44</v>
@@ -2866,13 +2927,13 @@
         <v>82</v>
       </c>
       <c r="F11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G11" t="s">
         <v>87</v>
       </c>
       <c r="H11" s="18">
-        <v>40902</v>
+        <v>40901</v>
       </c>
       <c r="I11" s="18">
         <v>40902</v>
@@ -2892,28 +2953,31 @@
     </row>
     <row r="12" spans="1:14">
       <c r="B12" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="C12" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D12" t="s">
-        <v>92</v>
+        <v>44</v>
       </c>
       <c r="E12" t="s">
         <v>82</v>
       </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
       <c r="G12" t="s">
         <v>87</v>
       </c>
       <c r="H12" s="18">
-        <v>40901</v>
+        <v>40902</v>
       </c>
       <c r="I12" s="18">
         <v>40902</v>
       </c>
       <c r="J12" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="K12" s="18">
         <v>40902</v>
@@ -2922,15 +2986,15 @@
         <v>87</v>
       </c>
       <c r="M12" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:14">
       <c r="B13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D13" t="s">
         <v>92</v>
@@ -2939,7 +3003,7 @@
         <v>82</v>
       </c>
       <c r="G13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H13" s="18">
         <v>40901</v>
@@ -2962,10 +3026,10 @@
     </row>
     <row r="14" spans="1:14">
       <c r="B14" t="s">
-        <v>98</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>99</v>
+        <v>97</v>
+      </c>
+      <c r="C14" t="s">
+        <v>97</v>
       </c>
       <c r="D14" t="s">
         <v>92</v>
@@ -2973,21 +3037,20 @@
       <c r="E14" t="s">
         <v>82</v>
       </c>
-      <c r="F14" s="18"/>
       <c r="G14" t="s">
         <v>87</v>
       </c>
       <c r="H14" s="18">
+        <v>40901</v>
+      </c>
+      <c r="I14" s="18">
         <v>40902</v>
-      </c>
-      <c r="I14" s="18">
-        <v>40903</v>
       </c>
       <c r="J14" t="s">
         <v>6</v>
       </c>
       <c r="K14" s="18">
-        <v>40903</v>
+        <v>40902</v>
       </c>
       <c r="L14" t="s">
         <v>87</v>
@@ -2998,13 +3061,13 @@
     </row>
     <row r="15" spans="1:14">
       <c r="B15" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D15" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E15" t="s">
         <v>82</v>
@@ -3014,76 +3077,86 @@
         <v>87</v>
       </c>
       <c r="H15" s="18">
-        <v>40901</v>
+        <v>40902</v>
       </c>
       <c r="I15" s="18">
-        <v>40901</v>
+        <v>40903</v>
       </c>
       <c r="J15" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K15" s="18">
-        <v>40902</v>
+        <v>40903</v>
       </c>
       <c r="L15" t="s">
         <v>87</v>
       </c>
       <c r="M15" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:14">
       <c r="B16" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E16" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="F16" s="18"/>
       <c r="G16" t="s">
         <v>87</v>
       </c>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
+      <c r="H16" s="18">
+        <v>40901</v>
+      </c>
+      <c r="I16" s="18">
+        <v>40901</v>
+      </c>
+      <c r="J16" t="s">
+        <v>8</v>
+      </c>
+      <c r="K16" s="18">
+        <v>40902</v>
+      </c>
+      <c r="L16" t="s">
+        <v>87</v>
+      </c>
+      <c r="M16" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="17" spans="2:11">
       <c r="B17" t="s">
-        <v>79</v>
-      </c>
-      <c r="C17" t="s">
-        <v>104</v>
+        <v>101</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>102</v>
       </c>
       <c r="D17" t="s">
         <v>92</v>
       </c>
       <c r="E17" t="s">
-        <v>82</v>
-      </c>
-      <c r="F17">
-        <v>3</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="F17" s="18"/>
       <c r="G17" t="s">
         <v>87</v>
       </c>
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
-      <c r="J17" t="s">
-        <v>8</v>
-      </c>
-      <c r="K17" s="18"/>
     </row>
     <row r="18" spans="2:11">
       <c r="B18" t="s">
         <v>79</v>
       </c>
       <c r="C18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D18" t="s">
         <v>92</v>
@@ -3092,18 +3165,28 @@
         <v>82</v>
       </c>
       <c r="F18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G18" t="s">
         <v>87</v>
       </c>
+      <c r="H18" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I18" s="18">
+        <v>40903</v>
+      </c>
+      <c r="J18" t="s">
+        <v>8</v>
+      </c>
+      <c r="K18" s="18"/>
     </row>
     <row r="19" spans="2:11">
       <c r="B19" t="s">
         <v>79</v>
       </c>
       <c r="C19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D19" t="s">
         <v>92</v>
@@ -3112,7 +3195,7 @@
         <v>82</v>
       </c>
       <c r="F19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G19" t="s">
         <v>87</v>
@@ -3123,7 +3206,7 @@
         <v>79</v>
       </c>
       <c r="C20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D20" t="s">
         <v>92</v>
@@ -3132,7 +3215,7 @@
         <v>82</v>
       </c>
       <c r="F20">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G20" t="s">
         <v>87</v>
@@ -3143,7 +3226,7 @@
         <v>79</v>
       </c>
       <c r="C21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D21" t="s">
         <v>92</v>
@@ -3152,7 +3235,7 @@
         <v>82</v>
       </c>
       <c r="F21">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G21" t="s">
         <v>87</v>
@@ -3163,7 +3246,7 @@
         <v>79</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>108</v>
       </c>
       <c r="D22" t="s">
         <v>92</v>
@@ -3172,7 +3255,7 @@
         <v>82</v>
       </c>
       <c r="F22">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G22" t="s">
         <v>87</v>
@@ -3183,7 +3266,7 @@
         <v>79</v>
       </c>
       <c r="C23" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="D23" t="s">
         <v>92</v>
@@ -3192,10 +3275,13 @@
         <v>82</v>
       </c>
       <c r="F23">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G23" t="s">
         <v>87</v>
+      </c>
+      <c r="H23" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="24" spans="2:11">
@@ -3203,7 +3289,7 @@
         <v>79</v>
       </c>
       <c r="C24" t="s">
-        <v>109</v>
+        <v>12</v>
       </c>
       <c r="D24" t="s">
         <v>92</v>
@@ -3212,7 +3298,7 @@
         <v>82</v>
       </c>
       <c r="F24">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G24" t="s">
         <v>87</v>
@@ -3223,16 +3309,16 @@
         <v>79</v>
       </c>
       <c r="C25" t="s">
-        <v>23</v>
+        <v>109</v>
       </c>
       <c r="D25" t="s">
         <v>92</v>
       </c>
       <c r="E25" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="F25">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G25" t="s">
         <v>87</v>
@@ -3243,7 +3329,7 @@
         <v>79</v>
       </c>
       <c r="C26" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D26" t="s">
         <v>92</v>
@@ -3252,7 +3338,7 @@
         <v>110</v>
       </c>
       <c r="F26">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G26" t="s">
         <v>87</v>
@@ -3263,16 +3349,16 @@
         <v>79</v>
       </c>
       <c r="C27" t="s">
-        <v>104</v>
+        <v>22</v>
       </c>
       <c r="D27" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E27" t="s">
-        <v>82</v>
+        <v>110</v>
       </c>
       <c r="F27">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="G27" t="s">
         <v>87</v>
@@ -3283,7 +3369,7 @@
         <v>79</v>
       </c>
       <c r="C28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D28" t="s">
         <v>94</v>
@@ -3292,7 +3378,7 @@
         <v>82</v>
       </c>
       <c r="F28">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G28" t="s">
         <v>87</v>
@@ -3303,7 +3389,7 @@
         <v>79</v>
       </c>
       <c r="C29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D29" t="s">
         <v>94</v>
@@ -3312,7 +3398,7 @@
         <v>82</v>
       </c>
       <c r="F29">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G29" t="s">
         <v>87</v>
@@ -3323,7 +3409,7 @@
         <v>79</v>
       </c>
       <c r="C30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D30" t="s">
         <v>94</v>
@@ -3332,7 +3418,7 @@
         <v>82</v>
       </c>
       <c r="F30">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G30" t="s">
         <v>87</v>
@@ -3343,7 +3429,7 @@
         <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D31" t="s">
         <v>94</v>
@@ -3352,7 +3438,7 @@
         <v>82</v>
       </c>
       <c r="F31">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G31" t="s">
         <v>87</v>
@@ -3363,7 +3449,7 @@
         <v>79</v>
       </c>
       <c r="C32" t="s">
-        <v>30</v>
+        <v>108</v>
       </c>
       <c r="D32" t="s">
         <v>94</v>
@@ -3372,7 +3458,7 @@
         <v>82</v>
       </c>
       <c r="F32">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G32" t="s">
         <v>87</v>
@@ -3383,7 +3469,7 @@
         <v>79</v>
       </c>
       <c r="C33" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="D33" t="s">
         <v>94</v>
@@ -3392,7 +3478,7 @@
         <v>82</v>
       </c>
       <c r="F33">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G33" t="s">
         <v>87</v>
@@ -3403,7 +3489,7 @@
         <v>79</v>
       </c>
       <c r="C34" t="s">
-        <v>109</v>
+        <v>12</v>
       </c>
       <c r="D34" t="s">
         <v>94</v>
@@ -3412,7 +3498,7 @@
         <v>82</v>
       </c>
       <c r="F34">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G34" t="s">
         <v>87</v>
@@ -3423,16 +3509,16 @@
         <v>79</v>
       </c>
       <c r="C35" t="s">
-        <v>23</v>
+        <v>109</v>
       </c>
       <c r="D35" t="s">
         <v>94</v>
       </c>
       <c r="E35" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="F35">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G35" t="s">
         <v>87</v>
@@ -3443,7 +3529,7 @@
         <v>79</v>
       </c>
       <c r="C36" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D36" t="s">
         <v>94</v>
@@ -3452,7 +3538,7 @@
         <v>110</v>
       </c>
       <c r="F36">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G36" t="s">
         <v>87</v>
@@ -3463,29 +3549,19 @@
         <v>79</v>
       </c>
       <c r="C37" t="s">
-        <v>104</v>
+        <v>22</v>
       </c>
       <c r="D37" t="s">
-        <v>44</v>
+        <v>94</v>
       </c>
       <c r="E37" t="s">
-        <v>82</v>
+        <v>110</v>
       </c>
       <c r="F37">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="G37" t="s">
         <v>87</v>
-      </c>
-      <c r="J37" t="s">
-        <v>9</v>
-      </c>
-      <c r="K37" s="18"/>
-      <c r="L37" t="s">
-        <v>87</v>
-      </c>
-      <c r="M37" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="38" spans="2:13">
@@ -3493,7 +3569,7 @@
         <v>79</v>
       </c>
       <c r="C38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D38" t="s">
         <v>44</v>
@@ -3502,7 +3578,7 @@
         <v>82</v>
       </c>
       <c r="F38">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G38" t="s">
         <v>87</v>
@@ -3523,7 +3599,7 @@
         <v>79</v>
       </c>
       <c r="C39" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D39" t="s">
         <v>44</v>
@@ -3532,7 +3608,7 @@
         <v>82</v>
       </c>
       <c r="F39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G39" t="s">
         <v>87</v>
@@ -3540,6 +3616,7 @@
       <c r="J39" t="s">
         <v>9</v>
       </c>
+      <c r="K39" s="18"/>
       <c r="L39" t="s">
         <v>87</v>
       </c>
@@ -3552,7 +3629,7 @@
         <v>79</v>
       </c>
       <c r="C40" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D40" t="s">
         <v>44</v>
@@ -3561,7 +3638,7 @@
         <v>82</v>
       </c>
       <c r="F40">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G40" t="s">
         <v>87</v>
@@ -3581,7 +3658,7 @@
         <v>79</v>
       </c>
       <c r="C41" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D41" t="s">
         <v>44</v>
@@ -3590,7 +3667,7 @@
         <v>82</v>
       </c>
       <c r="F41">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G41" t="s">
         <v>87</v>
@@ -3610,7 +3687,7 @@
         <v>79</v>
       </c>
       <c r="C42" t="s">
-        <v>30</v>
+        <v>108</v>
       </c>
       <c r="D42" t="s">
         <v>44</v>
@@ -3619,7 +3696,7 @@
         <v>82</v>
       </c>
       <c r="F42">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G42" t="s">
         <v>87</v>
@@ -3639,7 +3716,7 @@
         <v>79</v>
       </c>
       <c r="C43" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="D43" t="s">
         <v>44</v>
@@ -3648,7 +3725,7 @@
         <v>82</v>
       </c>
       <c r="F43">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G43" t="s">
         <v>87</v>
@@ -3668,7 +3745,7 @@
         <v>79</v>
       </c>
       <c r="C44" t="s">
-        <v>109</v>
+        <v>12</v>
       </c>
       <c r="D44" t="s">
         <v>44</v>
@@ -3677,7 +3754,7 @@
         <v>82</v>
       </c>
       <c r="F44">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G44" t="s">
         <v>87</v>
@@ -3697,16 +3774,16 @@
         <v>79</v>
       </c>
       <c r="C45" t="s">
-        <v>23</v>
+        <v>109</v>
       </c>
       <c r="D45" t="s">
         <v>44</v>
       </c>
       <c r="E45" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="F45">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G45" t="s">
         <v>87</v>
@@ -3726,7 +3803,7 @@
         <v>79</v>
       </c>
       <c r="C46" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D46" t="s">
         <v>44</v>
@@ -3735,7 +3812,7 @@
         <v>110</v>
       </c>
       <c r="F46">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G46" t="s">
         <v>87</v>
@@ -3752,22 +3829,31 @@
     </row>
     <row r="47" spans="2:13">
       <c r="B47" t="s">
-        <v>111</v>
+        <v>79</v>
       </c>
       <c r="C47" t="s">
-        <v>112</v>
+        <v>22</v>
       </c>
       <c r="D47" t="s">
-        <v>92</v>
+        <v>44</v>
       </c>
       <c r="E47" t="s">
-        <v>82</v>
+        <v>110</v>
       </c>
       <c r="F47">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G47" t="s">
         <v>87</v>
+      </c>
+      <c r="J47" t="s">
+        <v>9</v>
+      </c>
+      <c r="L47" t="s">
+        <v>87</v>
+      </c>
+      <c r="M47" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="2:13">
@@ -3775,7 +3861,7 @@
         <v>111</v>
       </c>
       <c r="C48" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D48" t="s">
         <v>92</v>
@@ -3784,7 +3870,7 @@
         <v>82</v>
       </c>
       <c r="F48">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G48" t="s">
         <v>87</v>
@@ -3795,7 +3881,7 @@
         <v>111</v>
       </c>
       <c r="C49" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D49" t="s">
         <v>92</v>
@@ -3804,7 +3890,7 @@
         <v>82</v>
       </c>
       <c r="F49">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G49" t="s">
         <v>87</v>
@@ -3815,7 +3901,7 @@
         <v>111</v>
       </c>
       <c r="C50" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D50" t="s">
         <v>92</v>
@@ -3824,7 +3910,7 @@
         <v>82</v>
       </c>
       <c r="F50">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G50" t="s">
         <v>87</v>
@@ -3835,7 +3921,7 @@
         <v>111</v>
       </c>
       <c r="C51" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="D51" t="s">
         <v>92</v>
@@ -3844,7 +3930,7 @@
         <v>82</v>
       </c>
       <c r="F51">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G51" t="s">
         <v>87</v>
@@ -3855,16 +3941,16 @@
         <v>111</v>
       </c>
       <c r="C52" t="s">
-        <v>18</v>
+        <v>106</v>
       </c>
       <c r="D52" t="s">
         <v>92</v>
       </c>
       <c r="E52" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="F52">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G52" t="s">
         <v>87</v>
@@ -3875,7 +3961,7 @@
         <v>111</v>
       </c>
       <c r="C53" t="s">
-        <v>116</v>
+        <v>18</v>
       </c>
       <c r="D53" t="s">
         <v>92</v>
@@ -3884,7 +3970,7 @@
         <v>103</v>
       </c>
       <c r="F53">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G53" t="s">
         <v>87</v>
@@ -3895,7 +3981,7 @@
         <v>111</v>
       </c>
       <c r="C54" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D54" t="s">
         <v>92</v>
@@ -3904,7 +3990,7 @@
         <v>103</v>
       </c>
       <c r="F54">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G54" t="s">
         <v>87</v>
@@ -3915,16 +4001,16 @@
         <v>111</v>
       </c>
       <c r="C55" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D55" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E55" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="F55">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G55" t="s">
         <v>87</v>
@@ -3935,7 +4021,7 @@
         <v>111</v>
       </c>
       <c r="C56" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D56" t="s">
         <v>94</v>
@@ -3944,7 +4030,7 @@
         <v>82</v>
       </c>
       <c r="F56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G56" t="s">
         <v>87</v>
@@ -3955,7 +4041,7 @@
         <v>111</v>
       </c>
       <c r="C57" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D57" t="s">
         <v>94</v>
@@ -3964,7 +4050,7 @@
         <v>82</v>
       </c>
       <c r="F57">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G57" t="s">
         <v>87</v>
@@ -3975,7 +4061,7 @@
         <v>111</v>
       </c>
       <c r="C58" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D58" t="s">
         <v>94</v>
@@ -3984,7 +4070,7 @@
         <v>82</v>
       </c>
       <c r="F58">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G58" t="s">
         <v>87</v>
@@ -3995,7 +4081,7 @@
         <v>111</v>
       </c>
       <c r="C59" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="D59" t="s">
         <v>94</v>
@@ -4004,7 +4090,7 @@
         <v>82</v>
       </c>
       <c r="F59">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G59" t="s">
         <v>87</v>
@@ -4015,16 +4101,16 @@
         <v>111</v>
       </c>
       <c r="C60" t="s">
-        <v>18</v>
+        <v>106</v>
       </c>
       <c r="D60" t="s">
         <v>94</v>
       </c>
       <c r="E60" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="F60">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G60" t="s">
         <v>87</v>
@@ -4035,7 +4121,7 @@
         <v>111</v>
       </c>
       <c r="C61" t="s">
-        <v>116</v>
+        <v>18</v>
       </c>
       <c r="D61" t="s">
         <v>94</v>
@@ -4044,7 +4130,7 @@
         <v>103</v>
       </c>
       <c r="F61">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G61" t="s">
         <v>87</v>
@@ -4055,7 +4141,7 @@
         <v>111</v>
       </c>
       <c r="C62" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D62" t="s">
         <v>94</v>
@@ -4064,7 +4150,7 @@
         <v>103</v>
       </c>
       <c r="F62">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G62" t="s">
         <v>87</v>
@@ -4075,29 +4161,19 @@
         <v>111</v>
       </c>
       <c r="C63" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D63" t="s">
-        <v>44</v>
+        <v>94</v>
       </c>
       <c r="E63" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="F63">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G63" t="s">
         <v>87</v>
-      </c>
-      <c r="J63" t="s">
-        <v>9</v>
-      </c>
-      <c r="K63" s="18"/>
-      <c r="L63" t="s">
-        <v>87</v>
-      </c>
-      <c r="M63" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="64" spans="2:13">
@@ -4105,7 +4181,7 @@
         <v>111</v>
       </c>
       <c r="C64" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D64" t="s">
         <v>44</v>
@@ -4114,7 +4190,7 @@
         <v>82</v>
       </c>
       <c r="F64">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G64" t="s">
         <v>87</v>
@@ -4135,7 +4211,7 @@
         <v>111</v>
       </c>
       <c r="C65" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D65" t="s">
         <v>44</v>
@@ -4144,7 +4220,7 @@
         <v>82</v>
       </c>
       <c r="F65">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G65" t="s">
         <v>87</v>
@@ -4152,6 +4228,7 @@
       <c r="J65" t="s">
         <v>9</v>
       </c>
+      <c r="K65" s="18"/>
       <c r="L65" t="s">
         <v>87</v>
       </c>
@@ -4164,7 +4241,7 @@
         <v>111</v>
       </c>
       <c r="C66" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D66" t="s">
         <v>44</v>
@@ -4173,7 +4250,7 @@
         <v>82</v>
       </c>
       <c r="F66">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G66" t="s">
         <v>87</v>
@@ -4193,7 +4270,7 @@
         <v>111</v>
       </c>
       <c r="C67" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="D67" t="s">
         <v>44</v>
@@ -4202,7 +4279,7 @@
         <v>82</v>
       </c>
       <c r="F67">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G67" t="s">
         <v>87</v>
@@ -4222,16 +4299,16 @@
         <v>111</v>
       </c>
       <c r="C68" t="s">
-        <v>18</v>
+        <v>106</v>
       </c>
       <c r="D68" t="s">
         <v>44</v>
       </c>
       <c r="E68" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="F68">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G68" t="s">
         <v>87</v>
@@ -4251,7 +4328,7 @@
         <v>111</v>
       </c>
       <c r="C69" t="s">
-        <v>116</v>
+        <v>18</v>
       </c>
       <c r="D69" t="s">
         <v>44</v>
@@ -4260,7 +4337,7 @@
         <v>103</v>
       </c>
       <c r="F69">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G69" t="s">
         <v>87</v>
@@ -4280,7 +4357,7 @@
         <v>111</v>
       </c>
       <c r="C70" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D70" t="s">
         <v>44</v>
@@ -4289,7 +4366,7 @@
         <v>103</v>
       </c>
       <c r="F70">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G70" t="s">
         <v>87</v>
@@ -4306,22 +4383,31 @@
     </row>
     <row r="71" spans="2:13">
       <c r="B71" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C71" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D71" t="s">
-        <v>92</v>
+        <v>44</v>
       </c>
       <c r="E71" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="F71">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G71" t="s">
         <v>87</v>
+      </c>
+      <c r="J71" t="s">
+        <v>9</v>
+      </c>
+      <c r="L71" t="s">
+        <v>87</v>
+      </c>
+      <c r="M71" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="72" spans="2:13">
@@ -4329,7 +4415,7 @@
         <v>118</v>
       </c>
       <c r="C72" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D72" t="s">
         <v>92</v>
@@ -4338,7 +4424,7 @@
         <v>82</v>
       </c>
       <c r="F72">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G72" t="s">
         <v>87</v>
@@ -4349,7 +4435,7 @@
         <v>118</v>
       </c>
       <c r="C73" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D73" t="s">
         <v>92</v>
@@ -4358,32 +4444,35 @@
         <v>82</v>
       </c>
       <c r="F73">
+        <v>2</v>
+      </c>
+      <c r="G73" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="74" spans="2:13">
+      <c r="B74" t="s">
+        <v>118</v>
+      </c>
+      <c r="C74" t="s">
+        <v>121</v>
+      </c>
+      <c r="D74" t="s">
+        <v>92</v>
+      </c>
+      <c r="E74" t="s">
+        <v>82</v>
+      </c>
+      <c r="F74">
         <v>3</v>
       </c>
-      <c r="G73" s="19" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="74" spans="2:13">
-      <c r="C74" t="s">
-        <v>119</v>
-      </c>
-      <c r="D74" t="s">
-        <v>94</v>
-      </c>
-      <c r="E74" t="s">
-        <v>82</v>
-      </c>
-      <c r="F74">
-        <v>1</v>
-      </c>
-      <c r="G74" t="s">
+      <c r="G74" s="19" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="75" spans="2:13">
       <c r="C75" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D75" t="s">
         <v>94</v>
@@ -4392,7 +4481,7 @@
         <v>82</v>
       </c>
       <c r="F75">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G75" t="s">
         <v>87</v>
@@ -4400,7 +4489,7 @@
     </row>
     <row r="76" spans="2:13">
       <c r="C76" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D76" t="s">
         <v>94</v>
@@ -4409,42 +4498,32 @@
         <v>82</v>
       </c>
       <c r="F76">
-        <v>3</v>
-      </c>
-      <c r="G76" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G76" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="77" spans="2:13">
       <c r="C77" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D77" t="s">
-        <v>44</v>
+        <v>94</v>
       </c>
       <c r="E77" t="s">
         <v>82</v>
       </c>
       <c r="F77">
-        <v>1</v>
-      </c>
-      <c r="G77" t="s">
-        <v>87</v>
-      </c>
-      <c r="J77" t="s">
-        <v>9</v>
-      </c>
-      <c r="K77" s="18"/>
-      <c r="L77" t="s">
-        <v>87</v>
-      </c>
-      <c r="M77" t="s">
-        <v>7</v>
+        <v>3</v>
+      </c>
+      <c r="G77" s="19" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="78" spans="2:13">
       <c r="C78" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D78" t="s">
         <v>44</v>
@@ -4453,7 +4532,7 @@
         <v>82</v>
       </c>
       <c r="F78">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G78" t="s">
         <v>87</v>
@@ -4471,7 +4550,7 @@
     </row>
     <row r="79" spans="2:13">
       <c r="C79" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D79" t="s">
         <v>44</v>
@@ -4480,14 +4559,15 @@
         <v>82</v>
       </c>
       <c r="F79">
-        <v>3</v>
-      </c>
-      <c r="G79" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G79" t="s">
         <v>87</v>
       </c>
       <c r="J79" t="s">
         <v>9</v>
       </c>
+      <c r="K79" s="18"/>
       <c r="L79" t="s">
         <v>87</v>
       </c>
@@ -4496,37 +4576,43 @@
       </c>
     </row>
     <row r="80" spans="2:13">
-      <c r="B80" t="s">
+      <c r="C80" t="s">
+        <v>121</v>
+      </c>
+      <c r="D80" t="s">
+        <v>44</v>
+      </c>
+      <c r="E80" t="s">
+        <v>82</v>
+      </c>
+      <c r="F80">
+        <v>3</v>
+      </c>
+      <c r="G80" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="J80" t="s">
+        <v>9</v>
+      </c>
+      <c r="L80" t="s">
+        <v>87</v>
+      </c>
+      <c r="M80" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="2:10">
+      <c r="B81" t="s">
         <v>101</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C81" t="s">
         <v>122</v>
-      </c>
-      <c r="D80" t="s">
-        <v>92</v>
-      </c>
-      <c r="E80" t="s">
-        <v>82</v>
-      </c>
-      <c r="F80">
-        <v>1</v>
-      </c>
-      <c r="G80" s="19" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="81" spans="2:13">
-      <c r="B81" t="s">
-        <v>123</v>
-      </c>
-      <c r="C81" t="s">
-        <v>124</v>
       </c>
       <c r="D81" t="s">
         <v>92</v>
       </c>
       <c r="E81" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="F81">
         <v>1</v>
@@ -4535,12 +4621,12 @@
         <v>87</v>
       </c>
     </row>
-    <row r="82" spans="2:13">
+    <row r="82" spans="2:10">
       <c r="B82" t="s">
         <v>123</v>
       </c>
       <c r="C82" t="s">
-        <v>32</v>
+        <v>124</v>
       </c>
       <c r="D82" t="s">
         <v>92</v>
@@ -4549,18 +4635,18 @@
         <v>110</v>
       </c>
       <c r="F82">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G82" s="19" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="83" spans="2:13">
+    <row r="83" spans="2:10">
       <c r="B83" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C83" t="s">
-        <v>126</v>
+        <v>32</v>
       </c>
       <c r="D83" t="s">
         <v>92</v>
@@ -4569,18 +4655,18 @@
         <v>110</v>
       </c>
       <c r="F83">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G83" s="19" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="84" spans="2:13">
+    <row r="84" spans="2:10">
       <c r="B84" t="s">
         <v>125</v>
       </c>
       <c r="C84" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D84" t="s">
         <v>92</v>
@@ -4589,18 +4675,18 @@
         <v>110</v>
       </c>
       <c r="F84">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G84" s="19" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="85" spans="2:13">
+    <row r="85" spans="2:10">
       <c r="B85" t="s">
         <v>125</v>
       </c>
       <c r="C85" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D85" t="s">
         <v>92</v>
@@ -4609,18 +4695,18 @@
         <v>110</v>
       </c>
       <c r="F85">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G85" s="19" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="86" spans="2:13">
+    <row r="86" spans="2:10">
       <c r="B86" t="s">
         <v>125</v>
       </c>
       <c r="C86" t="s">
-        <v>23</v>
+        <v>128</v>
       </c>
       <c r="D86" t="s">
         <v>92</v>
@@ -4629,18 +4715,18 @@
         <v>110</v>
       </c>
       <c r="F86">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G86" s="19" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="87" spans="2:13">
+    <row r="87" spans="2:10">
       <c r="B87" t="s">
         <v>125</v>
       </c>
       <c r="C87" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D87" t="s">
         <v>92</v>
@@ -4649,24 +4735,24 @@
         <v>110</v>
       </c>
       <c r="F87">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G87" s="19" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="88" spans="2:13">
+    <row r="88" spans="2:10">
       <c r="B88" t="s">
-        <v>81</v>
+        <v>125</v>
       </c>
       <c r="C88" t="s">
-        <v>129</v>
+        <v>22</v>
       </c>
       <c r="D88" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="E88" t="s">
-        <v>82</v>
+        <v>110</v>
       </c>
       <c r="F88">
         <v>1</v>
@@ -4674,63 +4760,22 @@
       <c r="G88" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="H88" s="18">
-        <v>40901</v>
-      </c>
-      <c r="I88" s="18">
-        <v>40901</v>
-      </c>
-      <c r="J88" t="s">
-        <v>39</v>
-      </c>
-      <c r="K88" s="18">
-        <v>40901</v>
-      </c>
-      <c r="L88" t="s">
-        <v>87</v>
-      </c>
-      <c r="M88" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="89" spans="2:13">
-      <c r="B89" t="s">
-        <v>130</v>
-      </c>
-      <c r="C89" t="s">
-        <v>131</v>
-      </c>
-      <c r="D89" t="s">
-        <v>130</v>
-      </c>
-      <c r="E89" t="s">
-        <v>82</v>
-      </c>
-      <c r="F89">
-        <v>2</v>
-      </c>
-      <c r="G89" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="J89" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="90" spans="2:13">
+    </row>
+    <row r="90" spans="2:10">
       <c r="B90" t="s">
         <v>130</v>
       </c>
       <c r="C90" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D90" t="s">
         <v>130</v>
       </c>
       <c r="E90" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="F90">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G90" s="19" t="s">
         <v>87</v>
@@ -4739,12 +4784,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="91" spans="2:13">
+    <row r="91" spans="2:10">
       <c r="B91" t="s">
         <v>130</v>
       </c>
       <c r="C91" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D91" t="s">
         <v>130</v>
@@ -4753,7 +4798,7 @@
         <v>103</v>
       </c>
       <c r="F91">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G91" s="19" t="s">
         <v>87</v>
@@ -4762,38 +4807,35 @@
         <v>7</v>
       </c>
     </row>
-    <row r="92" spans="2:13">
+    <row r="92" spans="2:10">
       <c r="B92" t="s">
         <v>130</v>
       </c>
       <c r="C92" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D92" t="s">
         <v>130</v>
       </c>
       <c r="E92" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="F92">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G92" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="H92" s="18">
-        <v>40901</v>
-      </c>
       <c r="J92" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="93" spans="2:13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="93" spans="2:10">
       <c r="B93" t="s">
         <v>130</v>
       </c>
       <c r="C93" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D93" t="s">
         <v>130</v>
@@ -4802,18 +4844,24 @@
         <v>82</v>
       </c>
       <c r="F93">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G93" s="19" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="94" spans="2:13">
+      <c r="H93" s="18">
+        <v>40901</v>
+      </c>
+      <c r="J93" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="94" spans="2:10">
       <c r="B94" t="s">
         <v>130</v>
       </c>
       <c r="C94" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D94" t="s">
         <v>130</v>
@@ -4822,18 +4870,18 @@
         <v>82</v>
       </c>
       <c r="F94">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G94" s="19" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="95" spans="2:13">
+    <row r="95" spans="2:10">
       <c r="B95" t="s">
         <v>130</v>
       </c>
       <c r="C95" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D95" t="s">
         <v>130</v>
@@ -4842,24 +4890,21 @@
         <v>82</v>
       </c>
       <c r="F95">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G95" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="J95" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="96" spans="2:13">
+    </row>
+    <row r="96" spans="2:10">
       <c r="B96" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="C96" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D96" t="s">
-        <v>92</v>
+        <v>130</v>
       </c>
       <c r="E96" t="s">
         <v>82</v>
@@ -4870,31 +4915,16 @@
       <c r="G96" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="H96" s="18">
-        <v>40901</v>
-      </c>
-      <c r="I96" s="18">
-        <v>40901</v>
-      </c>
       <c r="J96" t="s">
-        <v>8</v>
-      </c>
-      <c r="K96" s="18">
-        <v>40902</v>
-      </c>
-      <c r="L96" t="s">
-        <v>87</v>
-      </c>
-      <c r="M96" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="97" spans="2:10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="97" spans="2:13">
       <c r="B97" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="C97" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D97" t="s">
         <v>92</v>
@@ -4902,13 +4932,37 @@
       <c r="E97" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="98" spans="2:10">
+      <c r="F97">
+        <v>1</v>
+      </c>
+      <c r="G97" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="H97" s="18">
+        <v>40901</v>
+      </c>
+      <c r="I97" s="18">
+        <v>40901</v>
+      </c>
+      <c r="J97" t="s">
+        <v>8</v>
+      </c>
+      <c r="K97" s="18">
+        <v>40902</v>
+      </c>
+      <c r="L97" t="s">
+        <v>87</v>
+      </c>
+      <c r="M97" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="2:13">
       <c r="B98" t="s">
         <v>101</v>
       </c>
       <c r="C98" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D98" t="s">
         <v>92</v>
@@ -4917,31 +4971,45 @@
         <v>82</v>
       </c>
     </row>
-    <row r="99" spans="2:10">
+    <row r="99" spans="2:13">
       <c r="B99" t="s">
         <v>101</v>
       </c>
       <c r="C99" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D99" t="s">
         <v>92</v>
       </c>
       <c r="E99" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="100" spans="2:13">
+      <c r="B100" t="s">
+        <v>101</v>
+      </c>
+      <c r="C100" t="s">
+        <v>142</v>
+      </c>
+      <c r="D100" t="s">
+        <v>92</v>
+      </c>
+      <c r="E100" t="s">
         <v>110</v>
       </c>
-      <c r="F99">
+      <c r="F100">
         <v>1</v>
       </c>
-      <c r="G99" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="J99" t="s">
+      <c r="G100" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="J100" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N99"/>
+  <autoFilter ref="A1:N100"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -4954,10 +5022,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5036,6 +5104,9 @@
       <c r="A7">
         <v>6</v>
       </c>
+      <c r="B7" t="s">
+        <v>148</v>
+      </c>
       <c r="C7" t="s">
         <v>87</v>
       </c>
@@ -5044,6 +5115,9 @@
       <c r="A8">
         <v>7</v>
       </c>
+      <c r="B8" t="s">
+        <v>149</v>
+      </c>
       <c r="C8" t="s">
         <v>87</v>
       </c>
@@ -5052,6 +5126,9 @@
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="B9" t="s">
+        <v>150</v>
+      </c>
       <c r="C9" t="s">
         <v>87</v>
       </c>
@@ -5060,9 +5137,38 @@
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10" t="s">
+        <v>151</v>
+      </c>
+      <c r="C10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>152</v>
+      </c>
+      <c r="C11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>153</v>
+      </c>
+      <c r="C12" t="s">
+        <v>87</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Updates on the plan and status.
</commit_message>
<xml_diff>
--- a/docs/PM-1 Project Management/PM-1.2 Plans/PM-1.2.1 Project Plan/vms_implementation_plan_v0.1a.xlsx
+++ b/docs/PM-1 Project Management/PM-1.2 Plans/PM-1.2.1 Project Plan/vms_implementation_plan_v0.1a.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="25600" windowHeight="14320" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14320" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$51</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tasks!$A$1:$N$100</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tasks!$A$1:$N$113</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="161">
   <si>
     <t>No</t>
   </si>
@@ -641,9 +641,6 @@
     <t>Audit Log Meeting Minutes</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Validator</t>
   </si>
   <si>
@@ -660,6 +657,30 @@
   </si>
   <si>
     <t>Database Script</t>
+  </si>
+  <si>
+    <t>Peishan is just to confirm if Thida has sent out the design.</t>
+  </si>
+  <si>
+    <t>Test Case</t>
+  </si>
+  <si>
+    <t>Added DateUtil, StringUtil</t>
+  </si>
+  <si>
+    <t>Data Loading</t>
+  </si>
+  <si>
+    <t>http://static.springsource.org/spring/docs/2.5.x/reference/view.html#view-jsp-formtaglib-errorstag (14.4.5.2. Simple binding)</t>
+  </si>
+  <si>
+    <t>Upgrade Jasper Library to 4.1.2</t>
+  </si>
+  <si>
+    <t>Data Preparation</t>
+  </si>
+  <si>
+    <t>Dio, Jifa</t>
   </si>
 </sst>
 </file>
@@ -823,8 +844,248 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="287">
+  <cellStyleXfs count="527">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1147,7 +1408,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="287">
+  <cellStyles count="527">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1291,6 +1552,126 @@
     <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="322" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="324" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="326" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="328" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="330" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="332" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="334" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="336" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="338" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="340" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="342" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="344" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="346" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="348" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="350" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="352" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="354" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="356" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="358" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="360" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="362" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="364" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="366" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="368" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="370" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="372" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="374" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="376" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="378" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="380" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="382" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="384" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="386" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="388" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="390" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="392" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="394" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="396" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="398" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="400" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="402" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="404" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="406" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="408" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="410" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="412" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="414" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="416" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="418" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="420" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="422" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="424" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="426" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="428" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="430" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="432" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="434" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="436" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="438" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="440" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="442" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="444" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="446" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="448" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="450" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="452" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="454" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="456" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="458" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="460" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="462" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="464" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="466" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="468" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="470" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="472" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="474" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="476" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="478" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="480" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="482" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="484" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="486" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="488" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="490" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="492" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="494" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="496" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="498" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="500" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="502" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="504" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="506" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="508" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="510" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="512" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="514" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="516" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="518" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="520" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="522" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="524" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="526" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1434,6 +1815,126 @@
     <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="319" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="321" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="323" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="325" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="327" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="329" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="331" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="333" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="335" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="337" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="339" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="341" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="343" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="345" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="347" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="349" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="351" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="353" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="355" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="357" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="359" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="361" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="363" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="365" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="367" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="369" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="371" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="373" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="375" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="377" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="379" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="381" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="383" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="385" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="387" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="389" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="391" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="393" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="395" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="397" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="399" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="401" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="403" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="405" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="407" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="409" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="411" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="413" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="415" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="417" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="419" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="421" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="423" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="425" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="427" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="429" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="431" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="433" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="435" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="437" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="439" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="441" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="443" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="445" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="447" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="449" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="451" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="453" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="455" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="457" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="459" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="461" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="463" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="465" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="467" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="469" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="471" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="473" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="475" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="477" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="479" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="481" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="483" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="485" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="487" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="489" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="491" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="493" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="495" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="497" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="499" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="501" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="503" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="505" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="507" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="509" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="511" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="513" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="515" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="517" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="519" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="521" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="523" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="525" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2516,16 +3017,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N100"/>
+  <dimension ref="A1:N116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="57.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
@@ -2682,10 +3186,10 @@
         <v>40901</v>
       </c>
       <c r="L4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="M4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -2720,10 +3224,10 @@
         <v>40901</v>
       </c>
       <c r="L5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="M5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -2740,7 +3244,7 @@
         <v>82</v>
       </c>
       <c r="G6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H6" s="18">
         <v>40901</v>
@@ -2755,7 +3259,7 @@
         <v>40901</v>
       </c>
       <c r="L6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="M6" t="s">
         <v>6</v>
@@ -2778,7 +3282,7 @@
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H7" s="18">
         <v>40901</v>
@@ -2816,7 +3320,7 @@
         <v>2</v>
       </c>
       <c r="G8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H8" s="18">
         <v>40902</v>
@@ -2921,7 +3425,7 @@
         <v>91</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>154</v>
       </c>
       <c r="E11" t="s">
         <v>82</v>
@@ -2959,7 +3463,7 @@
         <v>93</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>154</v>
       </c>
       <c r="E12" t="s">
         <v>82</v>
@@ -3003,7 +3507,7 @@
         <v>82</v>
       </c>
       <c r="G13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H13" s="18">
         <v>40901</v>
@@ -3038,7 +3542,7 @@
         <v>82</v>
       </c>
       <c r="G14" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H14" s="18">
         <v>40901</v>
@@ -3077,16 +3581,16 @@
         <v>87</v>
       </c>
       <c r="H15" s="18">
-        <v>40902</v>
+        <v>40903</v>
       </c>
       <c r="I15" s="18">
-        <v>40903</v>
+        <v>40904</v>
       </c>
       <c r="J15" t="s">
         <v>6</v>
       </c>
       <c r="K15" s="18">
-        <v>40903</v>
+        <v>40905</v>
       </c>
       <c r="L15" t="s">
         <v>87</v>
@@ -3110,7 +3614,7 @@
       </c>
       <c r="F16" s="18"/>
       <c r="G16" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H16" s="18">
         <v>40901</v>
@@ -3122,13 +3626,16 @@
         <v>8</v>
       </c>
       <c r="K16" s="18">
-        <v>40902</v>
+        <v>40901</v>
       </c>
       <c r="L16" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="M16" t="s">
         <v>6</v>
+      </c>
+      <c r="N16" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="2:11">
@@ -3177,7 +3684,7 @@
         <v>40903</v>
       </c>
       <c r="J18" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="K18" s="18"/>
     </row>
@@ -3200,6 +3707,15 @@
       <c r="G19" t="s">
         <v>87</v>
       </c>
+      <c r="H19" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I19" s="18">
+        <v>40903</v>
+      </c>
+      <c r="J19" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="20" spans="2:11">
       <c r="B20" t="s">
@@ -3220,6 +3736,15 @@
       <c r="G20" t="s">
         <v>87</v>
       </c>
+      <c r="H20" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I20" s="18">
+        <v>40903</v>
+      </c>
+      <c r="J20" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="21" spans="2:11">
       <c r="B21" t="s">
@@ -3240,6 +3765,15 @@
       <c r="G21" t="s">
         <v>87</v>
       </c>
+      <c r="H21" s="18">
+        <v>40904</v>
+      </c>
+      <c r="I21" s="18">
+        <v>40904</v>
+      </c>
+      <c r="J21" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="22" spans="2:11">
       <c r="B22" t="s">
@@ -3260,6 +3794,15 @@
       <c r="G22" t="s">
         <v>87</v>
       </c>
+      <c r="H22" s="18">
+        <v>40905</v>
+      </c>
+      <c r="I22" s="18">
+        <v>40905</v>
+      </c>
+      <c r="J22" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="23" spans="2:11">
       <c r="B23" t="s">
@@ -3280,8 +3823,14 @@
       <c r="G23" t="s">
         <v>87</v>
       </c>
-      <c r="H23" t="s">
-        <v>147</v>
+      <c r="H23" s="18">
+        <v>40906</v>
+      </c>
+      <c r="I23" s="18">
+        <v>40906</v>
+      </c>
+      <c r="J23" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="2:11">
@@ -3303,6 +3852,15 @@
       <c r="G24" t="s">
         <v>87</v>
       </c>
+      <c r="H24" s="18">
+        <v>40907</v>
+      </c>
+      <c r="I24" s="18">
+        <v>40907</v>
+      </c>
+      <c r="J24" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="25" spans="2:11">
       <c r="B25" t="s">
@@ -3323,6 +3881,15 @@
       <c r="G25" t="s">
         <v>87</v>
       </c>
+      <c r="H25" s="18">
+        <v>40905</v>
+      </c>
+      <c r="I25" s="18">
+        <v>40905</v>
+      </c>
+      <c r="J25" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="26" spans="2:11">
       <c r="B26" t="s">
@@ -3343,6 +3910,15 @@
       <c r="G26" t="s">
         <v>87</v>
       </c>
+      <c r="H26" s="18">
+        <v>40906</v>
+      </c>
+      <c r="I26" s="18">
+        <v>40906</v>
+      </c>
+      <c r="J26" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="27" spans="2:11">
       <c r="B27" t="s">
@@ -3363,6 +3939,15 @@
       <c r="G27" t="s">
         <v>87</v>
       </c>
+      <c r="H27" s="18">
+        <v>40906</v>
+      </c>
+      <c r="I27" s="18">
+        <v>40906</v>
+      </c>
+      <c r="J27" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="28" spans="2:11">
       <c r="B28" t="s">
@@ -3383,6 +3968,15 @@
       <c r="G28" t="s">
         <v>87</v>
       </c>
+      <c r="H28" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I28" s="18">
+        <v>40903</v>
+      </c>
+      <c r="J28" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="29" spans="2:11">
       <c r="B29" t="s">
@@ -3403,6 +3997,15 @@
       <c r="G29" t="s">
         <v>87</v>
       </c>
+      <c r="H29" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I29" s="18">
+        <v>40903</v>
+      </c>
+      <c r="J29" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="30" spans="2:11">
       <c r="B30" t="s">
@@ -3423,6 +4026,15 @@
       <c r="G30" t="s">
         <v>87</v>
       </c>
+      <c r="H30" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I30" s="18">
+        <v>40903</v>
+      </c>
+      <c r="J30" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="31" spans="2:11">
       <c r="B31" t="s">
@@ -3443,6 +4055,15 @@
       <c r="G31" t="s">
         <v>87</v>
       </c>
+      <c r="H31" s="18">
+        <v>40904</v>
+      </c>
+      <c r="I31" s="18">
+        <v>40904</v>
+      </c>
+      <c r="J31" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="32" spans="2:11">
       <c r="B32" t="s">
@@ -3463,6 +4084,15 @@
       <c r="G32" t="s">
         <v>87</v>
       </c>
+      <c r="H32" s="18">
+        <v>40905</v>
+      </c>
+      <c r="I32" s="18">
+        <v>40905</v>
+      </c>
+      <c r="J32" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="33" spans="2:13">
       <c r="B33" t="s">
@@ -3483,6 +4113,15 @@
       <c r="G33" t="s">
         <v>87</v>
       </c>
+      <c r="H33" s="18">
+        <v>40906</v>
+      </c>
+      <c r="I33" s="18">
+        <v>40906</v>
+      </c>
+      <c r="J33" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="34" spans="2:13">
       <c r="B34" t="s">
@@ -3503,6 +4142,15 @@
       <c r="G34" t="s">
         <v>87</v>
       </c>
+      <c r="H34" s="18">
+        <v>40907</v>
+      </c>
+      <c r="I34" s="18">
+        <v>40907</v>
+      </c>
+      <c r="J34" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="35" spans="2:13">
       <c r="B35" t="s">
@@ -3523,6 +4171,15 @@
       <c r="G35" t="s">
         <v>87</v>
       </c>
+      <c r="H35" s="18">
+        <v>40905</v>
+      </c>
+      <c r="I35" s="18">
+        <v>40905</v>
+      </c>
+      <c r="J35" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="36" spans="2:13">
       <c r="B36" t="s">
@@ -3543,6 +4200,15 @@
       <c r="G36" t="s">
         <v>87</v>
       </c>
+      <c r="H36" s="18">
+        <v>40906</v>
+      </c>
+      <c r="I36" s="18">
+        <v>40906</v>
+      </c>
+      <c r="J36" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="37" spans="2:13">
       <c r="B37" t="s">
@@ -3563,6 +4229,15 @@
       <c r="G37" t="s">
         <v>87</v>
       </c>
+      <c r="H37" s="18">
+        <v>40906</v>
+      </c>
+      <c r="I37" s="18">
+        <v>40906</v>
+      </c>
+      <c r="J37" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="38" spans="2:13">
       <c r="B38" t="s">
@@ -3572,7 +4247,7 @@
         <v>104</v>
       </c>
       <c r="D38" t="s">
-        <v>44</v>
+        <v>154</v>
       </c>
       <c r="E38" t="s">
         <v>82</v>
@@ -3582,6 +4257,12 @@
       </c>
       <c r="G38" t="s">
         <v>87</v>
+      </c>
+      <c r="H38" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I38" s="18">
+        <v>40903</v>
       </c>
       <c r="J38" t="s">
         <v>9</v>
@@ -3602,7 +4283,7 @@
         <v>105</v>
       </c>
       <c r="D39" t="s">
-        <v>44</v>
+        <v>154</v>
       </c>
       <c r="E39" t="s">
         <v>82</v>
@@ -3612,6 +4293,12 @@
       </c>
       <c r="G39" t="s">
         <v>87</v>
+      </c>
+      <c r="H39" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I39" s="18">
+        <v>40903</v>
       </c>
       <c r="J39" t="s">
         <v>9</v>
@@ -3632,7 +4319,7 @@
         <v>106</v>
       </c>
       <c r="D40" t="s">
-        <v>44</v>
+        <v>154</v>
       </c>
       <c r="E40" t="s">
         <v>82</v>
@@ -3642,6 +4329,12 @@
       </c>
       <c r="G40" t="s">
         <v>87</v>
+      </c>
+      <c r="H40" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I40" s="18">
+        <v>40903</v>
       </c>
       <c r="J40" t="s">
         <v>9</v>
@@ -3661,7 +4354,7 @@
         <v>107</v>
       </c>
       <c r="D41" t="s">
-        <v>44</v>
+        <v>154</v>
       </c>
       <c r="E41" t="s">
         <v>82</v>
@@ -3671,6 +4364,12 @@
       </c>
       <c r="G41" t="s">
         <v>87</v>
+      </c>
+      <c r="H41" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I41" s="18">
+        <v>40903</v>
       </c>
       <c r="J41" t="s">
         <v>9</v>
@@ -3690,7 +4389,7 @@
         <v>108</v>
       </c>
       <c r="D42" t="s">
-        <v>44</v>
+        <v>154</v>
       </c>
       <c r="E42" t="s">
         <v>82</v>
@@ -3700,6 +4399,12 @@
       </c>
       <c r="G42" t="s">
         <v>87</v>
+      </c>
+      <c r="H42" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I42" s="18">
+        <v>40903</v>
       </c>
       <c r="J42" t="s">
         <v>9</v>
@@ -3719,7 +4424,7 @@
         <v>30</v>
       </c>
       <c r="D43" t="s">
-        <v>44</v>
+        <v>154</v>
       </c>
       <c r="E43" t="s">
         <v>82</v>
@@ -3729,6 +4434,12 @@
       </c>
       <c r="G43" t="s">
         <v>87</v>
+      </c>
+      <c r="H43" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I43" s="18">
+        <v>40903</v>
       </c>
       <c r="J43" t="s">
         <v>9</v>
@@ -3748,7 +4459,7 @@
         <v>12</v>
       </c>
       <c r="D44" t="s">
-        <v>44</v>
+        <v>154</v>
       </c>
       <c r="E44" t="s">
         <v>82</v>
@@ -3758,6 +4469,12 @@
       </c>
       <c r="G44" t="s">
         <v>87</v>
+      </c>
+      <c r="H44" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I44" s="18">
+        <v>40903</v>
       </c>
       <c r="J44" t="s">
         <v>9</v>
@@ -3777,7 +4494,7 @@
         <v>109</v>
       </c>
       <c r="D45" t="s">
-        <v>44</v>
+        <v>154</v>
       </c>
       <c r="E45" t="s">
         <v>82</v>
@@ -3787,6 +4504,12 @@
       </c>
       <c r="G45" t="s">
         <v>87</v>
+      </c>
+      <c r="H45" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I45" s="18">
+        <v>40903</v>
       </c>
       <c r="J45" t="s">
         <v>9</v>
@@ -3806,7 +4529,7 @@
         <v>23</v>
       </c>
       <c r="D46" t="s">
-        <v>44</v>
+        <v>154</v>
       </c>
       <c r="E46" t="s">
         <v>110</v>
@@ -3816,6 +4539,12 @@
       </c>
       <c r="G46" t="s">
         <v>87</v>
+      </c>
+      <c r="H46" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I46" s="18">
+        <v>40903</v>
       </c>
       <c r="J46" t="s">
         <v>9</v>
@@ -3835,7 +4564,7 @@
         <v>22</v>
       </c>
       <c r="D47" t="s">
-        <v>44</v>
+        <v>154</v>
       </c>
       <c r="E47" t="s">
         <v>110</v>
@@ -3845,6 +4574,12 @@
       </c>
       <c r="G47" t="s">
         <v>87</v>
+      </c>
+      <c r="H47" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I47" s="18">
+        <v>40903</v>
       </c>
       <c r="J47" t="s">
         <v>9</v>
@@ -3875,6 +4610,15 @@
       <c r="G48" t="s">
         <v>87</v>
       </c>
+      <c r="H48" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I48" s="18">
+        <v>40903</v>
+      </c>
+      <c r="J48" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="49" spans="2:13">
       <c r="B49" t="s">
@@ -3895,6 +4639,15 @@
       <c r="G49" t="s">
         <v>87</v>
       </c>
+      <c r="H49" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I49" s="18">
+        <v>40903</v>
+      </c>
+      <c r="J49" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="50" spans="2:13">
       <c r="B50" t="s">
@@ -3915,6 +4668,15 @@
       <c r="G50" t="s">
         <v>87</v>
       </c>
+      <c r="H50" s="18">
+        <v>40904</v>
+      </c>
+      <c r="I50" s="18">
+        <v>40904</v>
+      </c>
+      <c r="J50" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="51" spans="2:13">
       <c r="B51" t="s">
@@ -3935,6 +4697,15 @@
       <c r="G51" t="s">
         <v>87</v>
       </c>
+      <c r="H51" s="18">
+        <v>40905</v>
+      </c>
+      <c r="I51" s="18">
+        <v>40905</v>
+      </c>
+      <c r="J51" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="52" spans="2:13">
       <c r="B52" t="s">
@@ -3955,6 +4726,15 @@
       <c r="G52" t="s">
         <v>87</v>
       </c>
+      <c r="H52" s="18">
+        <v>40906</v>
+      </c>
+      <c r="I52" s="18">
+        <v>40906</v>
+      </c>
+      <c r="J52" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="53" spans="2:13">
       <c r="B53" t="s">
@@ -3975,6 +4755,8 @@
       <c r="G53" t="s">
         <v>87</v>
       </c>
+      <c r="H53" s="18"/>
+      <c r="I53" s="18"/>
     </row>
     <row r="54" spans="2:13">
       <c r="B54" t="s">
@@ -3995,6 +4777,8 @@
       <c r="G54" t="s">
         <v>87</v>
       </c>
+      <c r="H54" s="18"/>
+      <c r="I54" s="18"/>
     </row>
     <row r="55" spans="2:13">
       <c r="B55" t="s">
@@ -4035,6 +4819,15 @@
       <c r="G56" t="s">
         <v>87</v>
       </c>
+      <c r="H56" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I56" s="18">
+        <v>40903</v>
+      </c>
+      <c r="J56" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="57" spans="2:13">
       <c r="B57" t="s">
@@ -4055,6 +4848,15 @@
       <c r="G57" t="s">
         <v>87</v>
       </c>
+      <c r="H57" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I57" s="18">
+        <v>40903</v>
+      </c>
+      <c r="J57" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="58" spans="2:13">
       <c r="B58" t="s">
@@ -4075,6 +4877,15 @@
       <c r="G58" t="s">
         <v>87</v>
       </c>
+      <c r="H58" s="18">
+        <v>40904</v>
+      </c>
+      <c r="I58" s="18">
+        <v>40904</v>
+      </c>
+      <c r="J58" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="59" spans="2:13">
       <c r="B59" t="s">
@@ -4095,6 +4906,15 @@
       <c r="G59" t="s">
         <v>87</v>
       </c>
+      <c r="H59" s="18">
+        <v>40905</v>
+      </c>
+      <c r="I59" s="18">
+        <v>40905</v>
+      </c>
+      <c r="J59" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="60" spans="2:13">
       <c r="B60" t="s">
@@ -4115,6 +4935,15 @@
       <c r="G60" t="s">
         <v>87</v>
       </c>
+      <c r="H60" s="18">
+        <v>40906</v>
+      </c>
+      <c r="I60" s="18">
+        <v>40906</v>
+      </c>
+      <c r="J60" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="61" spans="2:13">
       <c r="B61" t="s">
@@ -4135,6 +4964,8 @@
       <c r="G61" t="s">
         <v>87</v>
       </c>
+      <c r="H61" s="18"/>
+      <c r="I61" s="18"/>
     </row>
     <row r="62" spans="2:13">
       <c r="B62" t="s">
@@ -4155,6 +4986,8 @@
       <c r="G62" t="s">
         <v>87</v>
       </c>
+      <c r="H62" s="18"/>
+      <c r="I62" s="18"/>
     </row>
     <row r="63" spans="2:13">
       <c r="B63" t="s">
@@ -4184,7 +5017,7 @@
         <v>112</v>
       </c>
       <c r="D64" t="s">
-        <v>44</v>
+        <v>154</v>
       </c>
       <c r="E64" t="s">
         <v>82</v>
@@ -4195,15 +5028,21 @@
       <c r="G64" t="s">
         <v>87</v>
       </c>
+      <c r="H64" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I64" s="18">
+        <v>40903</v>
+      </c>
       <c r="J64" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="K64" s="18"/>
       <c r="L64" t="s">
         <v>87</v>
       </c>
       <c r="M64" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65" spans="2:13">
@@ -4214,7 +5053,7 @@
         <v>113</v>
       </c>
       <c r="D65" t="s">
-        <v>44</v>
+        <v>154</v>
       </c>
       <c r="E65" t="s">
         <v>82</v>
@@ -4225,15 +5064,21 @@
       <c r="G65" t="s">
         <v>87</v>
       </c>
+      <c r="H65" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I65" s="18">
+        <v>40903</v>
+      </c>
       <c r="J65" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="K65" s="18"/>
       <c r="L65" t="s">
         <v>87</v>
       </c>
       <c r="M65" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="66" spans="2:13">
@@ -4244,7 +5089,7 @@
         <v>114</v>
       </c>
       <c r="D66" t="s">
-        <v>44</v>
+        <v>154</v>
       </c>
       <c r="E66" t="s">
         <v>82</v>
@@ -4255,14 +5100,20 @@
       <c r="G66" t="s">
         <v>87</v>
       </c>
+      <c r="H66" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I66" s="18">
+        <v>40903</v>
+      </c>
       <c r="J66" t="s">
+        <v>7</v>
+      </c>
+      <c r="L66" t="s">
+        <v>87</v>
+      </c>
+      <c r="M66" t="s">
         <v>9</v>
-      </c>
-      <c r="L66" t="s">
-        <v>87</v>
-      </c>
-      <c r="M66" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="67" spans="2:13">
@@ -4273,7 +5124,7 @@
         <v>115</v>
       </c>
       <c r="D67" t="s">
-        <v>44</v>
+        <v>154</v>
       </c>
       <c r="E67" t="s">
         <v>82</v>
@@ -4284,14 +5135,20 @@
       <c r="G67" t="s">
         <v>87</v>
       </c>
+      <c r="H67" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I67" s="18">
+        <v>40903</v>
+      </c>
       <c r="J67" t="s">
+        <v>7</v>
+      </c>
+      <c r="L67" t="s">
+        <v>87</v>
+      </c>
+      <c r="M67" t="s">
         <v>9</v>
-      </c>
-      <c r="L67" t="s">
-        <v>87</v>
-      </c>
-      <c r="M67" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="68" spans="2:13">
@@ -4302,7 +5159,7 @@
         <v>106</v>
       </c>
       <c r="D68" t="s">
-        <v>44</v>
+        <v>154</v>
       </c>
       <c r="E68" t="s">
         <v>82</v>
@@ -4313,14 +5170,20 @@
       <c r="G68" t="s">
         <v>87</v>
       </c>
+      <c r="H68" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I68" s="18">
+        <v>40903</v>
+      </c>
       <c r="J68" t="s">
+        <v>7</v>
+      </c>
+      <c r="L68" t="s">
+        <v>87</v>
+      </c>
+      <c r="M68" t="s">
         <v>9</v>
-      </c>
-      <c r="L68" t="s">
-        <v>87</v>
-      </c>
-      <c r="M68" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="69" spans="2:13">
@@ -4331,7 +5194,7 @@
         <v>18</v>
       </c>
       <c r="D69" t="s">
-        <v>44</v>
+        <v>154</v>
       </c>
       <c r="E69" t="s">
         <v>103</v>
@@ -4342,14 +5205,20 @@
       <c r="G69" t="s">
         <v>87</v>
       </c>
+      <c r="H69" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I69" s="18">
+        <v>40903</v>
+      </c>
       <c r="J69" t="s">
+        <v>7</v>
+      </c>
+      <c r="L69" t="s">
+        <v>87</v>
+      </c>
+      <c r="M69" t="s">
         <v>9</v>
-      </c>
-      <c r="L69" t="s">
-        <v>87</v>
-      </c>
-      <c r="M69" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="70" spans="2:13">
@@ -4360,7 +5229,7 @@
         <v>116</v>
       </c>
       <c r="D70" t="s">
-        <v>44</v>
+        <v>154</v>
       </c>
       <c r="E70" t="s">
         <v>103</v>
@@ -4371,14 +5240,20 @@
       <c r="G70" t="s">
         <v>87</v>
       </c>
+      <c r="H70" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I70" s="18">
+        <v>40903</v>
+      </c>
       <c r="J70" t="s">
+        <v>7</v>
+      </c>
+      <c r="L70" t="s">
+        <v>87</v>
+      </c>
+      <c r="M70" t="s">
         <v>9</v>
-      </c>
-      <c r="L70" t="s">
-        <v>87</v>
-      </c>
-      <c r="M70" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="71" spans="2:13">
@@ -4389,7 +5264,7 @@
         <v>117</v>
       </c>
       <c r="D71" t="s">
-        <v>44</v>
+        <v>154</v>
       </c>
       <c r="E71" t="s">
         <v>103</v>
@@ -4400,14 +5275,20 @@
       <c r="G71" t="s">
         <v>87</v>
       </c>
+      <c r="H71" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I71" s="18">
+        <v>40903</v>
+      </c>
       <c r="J71" t="s">
+        <v>7</v>
+      </c>
+      <c r="L71" t="s">
+        <v>87</v>
+      </c>
+      <c r="M71" t="s">
         <v>9</v>
-      </c>
-      <c r="L71" t="s">
-        <v>87</v>
-      </c>
-      <c r="M71" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="72" spans="2:13">
@@ -4429,6 +5310,15 @@
       <c r="G72" t="s">
         <v>87</v>
       </c>
+      <c r="H72" s="18">
+        <v>40904</v>
+      </c>
+      <c r="I72" s="18">
+        <v>40904</v>
+      </c>
+      <c r="J72" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="73" spans="2:13">
       <c r="B73" t="s">
@@ -4449,6 +5339,15 @@
       <c r="G73" t="s">
         <v>87</v>
       </c>
+      <c r="H73" s="18">
+        <v>40905</v>
+      </c>
+      <c r="I73" s="18">
+        <v>40905</v>
+      </c>
+      <c r="J73" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="74" spans="2:13">
       <c r="B74" t="s">
@@ -4469,8 +5368,20 @@
       <c r="G74" s="19" t="s">
         <v>87</v>
       </c>
+      <c r="H74" s="18">
+        <v>40906</v>
+      </c>
+      <c r="I74" s="18">
+        <v>40906</v>
+      </c>
+      <c r="J74" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="75" spans="2:13">
+      <c r="B75" t="s">
+        <v>118</v>
+      </c>
       <c r="C75" t="s">
         <v>119</v>
       </c>
@@ -4486,8 +5397,20 @@
       <c r="G75" t="s">
         <v>87</v>
       </c>
+      <c r="H75" s="18">
+        <v>40904</v>
+      </c>
+      <c r="I75" s="18">
+        <v>40904</v>
+      </c>
+      <c r="J75" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="76" spans="2:13">
+      <c r="B76" t="s">
+        <v>118</v>
+      </c>
       <c r="C76" t="s">
         <v>120</v>
       </c>
@@ -4503,8 +5426,20 @@
       <c r="G76" t="s">
         <v>87</v>
       </c>
+      <c r="H76" s="18">
+        <v>40905</v>
+      </c>
+      <c r="I76" s="18">
+        <v>40905</v>
+      </c>
+      <c r="J76" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="77" spans="2:13">
+      <c r="B77" t="s">
+        <v>118</v>
+      </c>
       <c r="C77" t="s">
         <v>121</v>
       </c>
@@ -4520,13 +5455,25 @@
       <c r="G77" s="19" t="s">
         <v>87</v>
       </c>
+      <c r="H77" s="18">
+        <v>40906</v>
+      </c>
+      <c r="I77" s="18">
+        <v>40906</v>
+      </c>
+      <c r="J77" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="78" spans="2:13">
+      <c r="B78" t="s">
+        <v>118</v>
+      </c>
       <c r="C78" t="s">
         <v>119</v>
       </c>
       <c r="D78" t="s">
-        <v>44</v>
+        <v>154</v>
       </c>
       <c r="E78" t="s">
         <v>82</v>
@@ -4537,6 +5484,12 @@
       <c r="G78" t="s">
         <v>87</v>
       </c>
+      <c r="H78" s="18">
+        <v>40904</v>
+      </c>
+      <c r="I78" s="18">
+        <v>40904</v>
+      </c>
       <c r="J78" t="s">
         <v>9</v>
       </c>
@@ -4549,11 +5502,14 @@
       </c>
     </row>
     <row r="79" spans="2:13">
+      <c r="B79" t="s">
+        <v>118</v>
+      </c>
       <c r="C79" t="s">
         <v>120</v>
       </c>
       <c r="D79" t="s">
-        <v>44</v>
+        <v>154</v>
       </c>
       <c r="E79" t="s">
         <v>82</v>
@@ -4564,6 +5520,12 @@
       <c r="G79" t="s">
         <v>87</v>
       </c>
+      <c r="H79" s="18">
+        <v>40904</v>
+      </c>
+      <c r="I79" s="18">
+        <v>40904</v>
+      </c>
       <c r="J79" t="s">
         <v>9</v>
       </c>
@@ -4576,11 +5538,14 @@
       </c>
     </row>
     <row r="80" spans="2:13">
+      <c r="B80" t="s">
+        <v>118</v>
+      </c>
       <c r="C80" t="s">
         <v>121</v>
       </c>
       <c r="D80" t="s">
-        <v>44</v>
+        <v>154</v>
       </c>
       <c r="E80" t="s">
         <v>82</v>
@@ -4591,6 +5556,12 @@
       <c r="G80" s="19" t="s">
         <v>87</v>
       </c>
+      <c r="H80" s="18">
+        <v>40904</v>
+      </c>
+      <c r="I80" s="18">
+        <v>40904</v>
+      </c>
       <c r="J80" t="s">
         <v>9</v>
       </c>
@@ -4601,7 +5572,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="2:10">
+    <row r="81" spans="2:13">
       <c r="B81" t="s">
         <v>101</v>
       </c>
@@ -4612,7 +5583,7 @@
         <v>92</v>
       </c>
       <c r="E81" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="F81">
         <v>1</v>
@@ -4621,7 +5592,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="82" spans="2:10">
+    <row r="82" spans="2:13">
       <c r="B82" t="s">
         <v>123</v>
       </c>
@@ -4640,8 +5611,13 @@
       <c r="G82" s="19" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="83" spans="2:10">
+      <c r="H82" s="18"/>
+      <c r="I82" s="18"/>
+      <c r="J82" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83" spans="2:13">
       <c r="B83" t="s">
         <v>123</v>
       </c>
@@ -4660,16 +5636,21 @@
       <c r="G83" s="19" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="84" spans="2:10">
+      <c r="H83" s="18"/>
+      <c r="I83" s="18"/>
+      <c r="J83" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84" spans="2:13">
       <c r="B84" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C84" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D84" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E84" t="s">
         <v>110</v>
@@ -4680,16 +5661,21 @@
       <c r="G84" s="19" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="85" spans="2:10">
+      <c r="H84" s="18"/>
+      <c r="I84" s="18"/>
+      <c r="J84" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="85" spans="2:13">
       <c r="B85" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C85" t="s">
-        <v>127</v>
+        <v>32</v>
       </c>
       <c r="D85" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E85" t="s">
         <v>110</v>
@@ -4700,53 +5686,88 @@
       <c r="G85" s="19" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="86" spans="2:10">
+      <c r="H85" s="18"/>
+      <c r="I85" s="18"/>
+      <c r="J85" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="86" spans="2:13">
       <c r="B86" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C86" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D86" t="s">
-        <v>92</v>
+        <v>154</v>
       </c>
       <c r="E86" t="s">
         <v>110</v>
       </c>
       <c r="F86">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G86" s="19" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="87" spans="2:10">
+      <c r="H86" s="18">
+        <v>40904</v>
+      </c>
+      <c r="I86" s="18">
+        <v>40904</v>
+      </c>
+      <c r="J86" t="s">
+        <v>7</v>
+      </c>
+      <c r="L86" t="s">
+        <v>87</v>
+      </c>
+      <c r="M86" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="87" spans="2:13">
       <c r="B87" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C87" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D87" t="s">
-        <v>92</v>
+        <v>154</v>
       </c>
       <c r="E87" t="s">
         <v>110</v>
       </c>
       <c r="F87">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G87" s="19" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="88" spans="2:10">
+      <c r="H87" s="18">
+        <v>40904</v>
+      </c>
+      <c r="I87" s="18">
+        <v>40904</v>
+      </c>
+      <c r="J87" t="s">
+        <v>7</v>
+      </c>
+      <c r="L87" t="s">
+        <v>87</v>
+      </c>
+      <c r="M87" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="88" spans="2:13">
       <c r="B88" t="s">
         <v>125</v>
       </c>
       <c r="C88" t="s">
-        <v>22</v>
+        <v>126</v>
       </c>
       <c r="D88" t="s">
         <v>92</v>
@@ -4760,134 +5781,202 @@
       <c r="G88" s="19" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="90" spans="2:10">
+      <c r="H88" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I88" s="18">
+        <v>40903</v>
+      </c>
+      <c r="J88" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="89" spans="2:13">
+      <c r="B89" t="s">
+        <v>125</v>
+      </c>
+      <c r="C89" t="s">
+        <v>127</v>
+      </c>
+      <c r="D89" t="s">
+        <v>92</v>
+      </c>
+      <c r="E89" t="s">
+        <v>110</v>
+      </c>
+      <c r="F89">
+        <v>2</v>
+      </c>
+      <c r="G89" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="H89" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I89" s="18">
+        <v>40903</v>
+      </c>
+      <c r="J89" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="90" spans="2:13">
       <c r="B90" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C90" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D90" t="s">
-        <v>130</v>
+        <v>92</v>
       </c>
       <c r="E90" t="s">
-        <v>82</v>
+        <v>110</v>
       </c>
       <c r="F90">
+        <v>3</v>
+      </c>
+      <c r="G90" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="H90" s="18">
+        <v>40904</v>
+      </c>
+      <c r="I90" s="18">
+        <v>40904</v>
+      </c>
+      <c r="J90" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="91" spans="2:13">
+      <c r="B91" t="s">
+        <v>125</v>
+      </c>
+      <c r="C91" t="s">
+        <v>23</v>
+      </c>
+      <c r="D91" t="s">
+        <v>92</v>
+      </c>
+      <c r="E91" t="s">
+        <v>110</v>
+      </c>
+      <c r="F91">
+        <v>4</v>
+      </c>
+      <c r="G91" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="H91" s="18">
+        <v>40905</v>
+      </c>
+      <c r="I91" s="18">
+        <v>40905</v>
+      </c>
+      <c r="J91" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="92" spans="2:13">
+      <c r="B92" t="s">
+        <v>125</v>
+      </c>
+      <c r="C92" t="s">
+        <v>22</v>
+      </c>
+      <c r="D92" t="s">
+        <v>92</v>
+      </c>
+      <c r="E92" t="s">
+        <v>110</v>
+      </c>
+      <c r="F92">
+        <v>5</v>
+      </c>
+      <c r="G92" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="H92" s="18">
+        <v>40906</v>
+      </c>
+      <c r="I92" s="18">
+        <v>40906</v>
+      </c>
+      <c r="J92" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93" spans="2:13">
+      <c r="B93" t="s">
+        <v>125</v>
+      </c>
+      <c r="C93" t="s">
+        <v>126</v>
+      </c>
+      <c r="D93" t="s">
+        <v>94</v>
+      </c>
+      <c r="E93" t="s">
+        <v>110</v>
+      </c>
+      <c r="F93">
+        <v>1</v>
+      </c>
+      <c r="G93" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="H93" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I93" s="18">
+        <v>40903</v>
+      </c>
+      <c r="J93" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="94" spans="2:13">
+      <c r="B94" t="s">
+        <v>125</v>
+      </c>
+      <c r="C94" t="s">
+        <v>127</v>
+      </c>
+      <c r="D94" t="s">
+        <v>94</v>
+      </c>
+      <c r="E94" t="s">
+        <v>110</v>
+      </c>
+      <c r="F94">
         <v>2</v>
       </c>
-      <c r="G90" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="J90" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="91" spans="2:10">
-      <c r="B91" t="s">
-        <v>130</v>
-      </c>
-      <c r="C91" t="s">
-        <v>132</v>
-      </c>
-      <c r="D91" t="s">
-        <v>130</v>
-      </c>
-      <c r="E91" t="s">
-        <v>103</v>
-      </c>
-      <c r="F91">
-        <v>6</v>
-      </c>
-      <c r="G91" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="J91" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="92" spans="2:10">
-      <c r="B92" t="s">
-        <v>130</v>
-      </c>
-      <c r="C92" t="s">
-        <v>133</v>
-      </c>
-      <c r="D92" t="s">
-        <v>130</v>
-      </c>
-      <c r="E92" t="s">
-        <v>103</v>
-      </c>
-      <c r="F92">
-        <v>7</v>
-      </c>
-      <c r="G92" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="J92" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="93" spans="2:10">
-      <c r="B93" t="s">
-        <v>130</v>
-      </c>
-      <c r="C93" t="s">
-        <v>134</v>
-      </c>
-      <c r="D93" t="s">
-        <v>130</v>
-      </c>
-      <c r="E93" t="s">
-        <v>82</v>
-      </c>
-      <c r="F93">
-        <v>4</v>
-      </c>
-      <c r="G93" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="H93" s="18">
-        <v>40901</v>
-      </c>
-      <c r="J93" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="94" spans="2:10">
-      <c r="B94" t="s">
-        <v>130</v>
-      </c>
-      <c r="C94" t="s">
-        <v>136</v>
-      </c>
-      <c r="D94" t="s">
-        <v>130</v>
-      </c>
-      <c r="E94" t="s">
-        <v>82</v>
-      </c>
-      <c r="F94">
-        <v>5</v>
-      </c>
       <c r="G94" s="19" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="95" spans="2:10">
+      <c r="H94" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I94" s="18">
+        <v>40903</v>
+      </c>
+      <c r="J94" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="95" spans="2:13">
       <c r="B95" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C95" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="D95" t="s">
-        <v>130</v>
+        <v>94</v>
       </c>
       <c r="E95" t="s">
-        <v>82</v>
+        <v>110</v>
       </c>
       <c r="F95">
         <v>3</v>
@@ -4895,121 +5984,579 @@
       <c r="G95" s="19" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="96" spans="2:10">
+      <c r="H95" s="18">
+        <v>40904</v>
+      </c>
+      <c r="I95" s="18">
+        <v>40904</v>
+      </c>
+      <c r="J95" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="96" spans="2:13">
       <c r="B96" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C96" t="s">
-        <v>138</v>
+        <v>23</v>
       </c>
       <c r="D96" t="s">
-        <v>130</v>
+        <v>94</v>
       </c>
       <c r="E96" t="s">
-        <v>82</v>
+        <v>110</v>
       </c>
       <c r="F96">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G96" s="19" t="s">
         <v>87</v>
       </c>
+      <c r="H96" s="18">
+        <v>40905</v>
+      </c>
+      <c r="I96" s="18">
+        <v>40905</v>
+      </c>
       <c r="J96" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="97" spans="2:13">
       <c r="B97" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C97" t="s">
-        <v>139</v>
+        <v>22</v>
       </c>
       <c r="D97" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E97" t="s">
-        <v>82</v>
+        <v>110</v>
       </c>
       <c r="F97">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G97" s="19" t="s">
         <v>87</v>
       </c>
       <c r="H97" s="18">
-        <v>40901</v>
+        <v>40906</v>
       </c>
       <c r="I97" s="18">
-        <v>40901</v>
+        <v>40906</v>
       </c>
       <c r="J97" t="s">
-        <v>8</v>
-      </c>
-      <c r="K97" s="18">
-        <v>40902</v>
-      </c>
-      <c r="L97" t="s">
-        <v>87</v>
-      </c>
-      <c r="M97" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="98" spans="2:13">
       <c r="B98" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="C98" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="D98" t="s">
-        <v>92</v>
+        <v>154</v>
       </c>
       <c r="E98" t="s">
-        <v>82</v>
+        <v>110</v>
+      </c>
+      <c r="F98">
+        <v>1</v>
+      </c>
+      <c r="G98" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="H98" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I98" s="18">
+        <v>40903</v>
+      </c>
+      <c r="J98" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="99" spans="2:13">
       <c r="B99" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="C99" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="D99" t="s">
-        <v>92</v>
+        <v>154</v>
       </c>
       <c r="E99" t="s">
-        <v>82</v>
+        <v>110</v>
+      </c>
+      <c r="F99">
+        <v>2</v>
+      </c>
+      <c r="G99" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="H99" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I99" s="18">
+        <v>40903</v>
+      </c>
+      <c r="J99" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="100" spans="2:13">
       <c r="B100" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="C100" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="D100" t="s">
-        <v>92</v>
+        <v>154</v>
       </c>
       <c r="E100" t="s">
         <v>110</v>
       </c>
       <c r="F100">
+        <v>3</v>
+      </c>
+      <c r="G100" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="H100" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I100" s="18">
+        <v>40903</v>
+      </c>
+      <c r="J100" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="101" spans="2:13">
+      <c r="B101" t="s">
+        <v>125</v>
+      </c>
+      <c r="C101" t="s">
+        <v>23</v>
+      </c>
+      <c r="D101" t="s">
+        <v>154</v>
+      </c>
+      <c r="E101" t="s">
+        <v>110</v>
+      </c>
+      <c r="F101">
+        <v>4</v>
+      </c>
+      <c r="G101" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="H101" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I101" s="18">
+        <v>40903</v>
+      </c>
+      <c r="J101" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102" spans="2:13">
+      <c r="B102" t="s">
+        <v>125</v>
+      </c>
+      <c r="C102" t="s">
+        <v>22</v>
+      </c>
+      <c r="D102" t="s">
+        <v>154</v>
+      </c>
+      <c r="E102" t="s">
+        <v>110</v>
+      </c>
+      <c r="F102">
+        <v>5</v>
+      </c>
+      <c r="G102" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="H102" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I102" s="18">
+        <v>40903</v>
+      </c>
+      <c r="J102" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="103" spans="2:13">
+      <c r="B103" t="s">
+        <v>130</v>
+      </c>
+      <c r="C103" t="s">
+        <v>131</v>
+      </c>
+      <c r="D103" t="s">
+        <v>130</v>
+      </c>
+      <c r="E103" t="s">
+        <v>82</v>
+      </c>
+      <c r="F103">
+        <v>2</v>
+      </c>
+      <c r="G103" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="H103" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I103" s="18">
+        <v>40903</v>
+      </c>
+      <c r="J103" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="104" spans="2:13">
+      <c r="B104" t="s">
+        <v>130</v>
+      </c>
+      <c r="C104" t="s">
+        <v>132</v>
+      </c>
+      <c r="D104" t="s">
+        <v>130</v>
+      </c>
+      <c r="E104" t="s">
+        <v>103</v>
+      </c>
+      <c r="F104">
+        <v>6</v>
+      </c>
+      <c r="G104" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="H104" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I104" s="18">
+        <v>40903</v>
+      </c>
+      <c r="J104" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="105" spans="2:13">
+      <c r="B105" t="s">
+        <v>130</v>
+      </c>
+      <c r="C105" t="s">
+        <v>133</v>
+      </c>
+      <c r="D105" t="s">
+        <v>130</v>
+      </c>
+      <c r="E105" t="s">
+        <v>103</v>
+      </c>
+      <c r="F105">
+        <v>7</v>
+      </c>
+      <c r="G105" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="H105" s="18">
+        <v>40903</v>
+      </c>
+      <c r="I105" s="18">
+        <v>40903</v>
+      </c>
+      <c r="J105" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="106" spans="2:13">
+      <c r="B106" t="s">
+        <v>130</v>
+      </c>
+      <c r="C106" t="s">
+        <v>134</v>
+      </c>
+      <c r="D106" t="s">
+        <v>130</v>
+      </c>
+      <c r="E106" t="s">
+        <v>82</v>
+      </c>
+      <c r="F106">
+        <v>4</v>
+      </c>
+      <c r="G106" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="H106" s="18">
+        <v>40901</v>
+      </c>
+      <c r="J106" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="107" spans="2:13">
+      <c r="B107" t="s">
+        <v>130</v>
+      </c>
+      <c r="C107" t="s">
+        <v>136</v>
+      </c>
+      <c r="D107" t="s">
+        <v>130</v>
+      </c>
+      <c r="E107" t="s">
+        <v>82</v>
+      </c>
+      <c r="F107">
+        <v>5</v>
+      </c>
+      <c r="G107" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="J107" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="108" spans="2:13">
+      <c r="B108" t="s">
+        <v>130</v>
+      </c>
+      <c r="C108" t="s">
+        <v>137</v>
+      </c>
+      <c r="D108" t="s">
+        <v>130</v>
+      </c>
+      <c r="E108" t="s">
+        <v>82</v>
+      </c>
+      <c r="F108">
+        <v>3</v>
+      </c>
+      <c r="G108" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="J108" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="109" spans="2:13">
+      <c r="B109" t="s">
+        <v>130</v>
+      </c>
+      <c r="C109" t="s">
+        <v>138</v>
+      </c>
+      <c r="D109" t="s">
+        <v>130</v>
+      </c>
+      <c r="E109" t="s">
+        <v>82</v>
+      </c>
+      <c r="F109">
         <v>1</v>
       </c>
-      <c r="G100" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="J100" t="s">
+      <c r="G109" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="J109" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="110" spans="2:13">
+      <c r="B110" t="s">
+        <v>123</v>
+      </c>
+      <c r="C110" t="s">
+        <v>139</v>
+      </c>
+      <c r="D110" t="s">
+        <v>92</v>
+      </c>
+      <c r="E110" t="s">
+        <v>82</v>
+      </c>
+      <c r="F110">
+        <v>1</v>
+      </c>
+      <c r="G110" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="H110" s="18">
+        <v>40901</v>
+      </c>
+      <c r="I110" s="18">
+        <v>40901</v>
+      </c>
+      <c r="J110" t="s">
+        <v>8</v>
+      </c>
+      <c r="K110" s="18">
+        <v>40902</v>
+      </c>
+      <c r="L110" t="s">
+        <v>87</v>
+      </c>
+      <c r="M110" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="111" spans="2:13">
+      <c r="B111" t="s">
+        <v>101</v>
+      </c>
+      <c r="C111" t="s">
+        <v>140</v>
+      </c>
+      <c r="D111" t="s">
+        <v>92</v>
+      </c>
+      <c r="E111" t="s">
+        <v>82</v>
+      </c>
+      <c r="F111">
+        <v>1</v>
+      </c>
+      <c r="G111" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="J111" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="112" spans="2:13">
+      <c r="B112" t="s">
+        <v>101</v>
+      </c>
+      <c r="C112" t="s">
+        <v>141</v>
+      </c>
+      <c r="D112" t="s">
+        <v>92</v>
+      </c>
+      <c r="E112" t="s">
+        <v>82</v>
+      </c>
+      <c r="F112">
+        <v>2</v>
+      </c>
+      <c r="G112" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="J112" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="113" spans="2:10">
+      <c r="B113" t="s">
+        <v>101</v>
+      </c>
+      <c r="C113" t="s">
+        <v>142</v>
+      </c>
+      <c r="D113" t="s">
+        <v>92</v>
+      </c>
+      <c r="E113" t="s">
+        <v>110</v>
+      </c>
+      <c r="F113">
+        <v>1</v>
+      </c>
+      <c r="G113" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="J113" t="s">
         <v>39</v>
       </c>
     </row>
+    <row r="114" spans="2:10">
+      <c r="B114" t="s">
+        <v>101</v>
+      </c>
+      <c r="C114" t="s">
+        <v>158</v>
+      </c>
+      <c r="D114" t="s">
+        <v>92</v>
+      </c>
+      <c r="E114" t="s">
+        <v>82</v>
+      </c>
+      <c r="F114">
+        <v>1</v>
+      </c>
+      <c r="G114" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="H114" s="18">
+        <v>40901</v>
+      </c>
+      <c r="I114" s="18">
+        <v>40901</v>
+      </c>
+      <c r="J114" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="115" spans="2:10">
+      <c r="C115" t="s">
+        <v>159</v>
+      </c>
+      <c r="D115" t="s">
+        <v>81</v>
+      </c>
+      <c r="E115" t="s">
+        <v>82</v>
+      </c>
+      <c r="G115" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="J115" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="116" spans="2:10">
+      <c r="C116" t="s">
+        <v>148</v>
+      </c>
+      <c r="D116" t="s">
+        <v>92</v>
+      </c>
+      <c r="E116" t="s">
+        <v>82</v>
+      </c>
+      <c r="G116" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="H116" s="18">
+        <v>40901</v>
+      </c>
+      <c r="I116" s="18">
+        <v>40901</v>
+      </c>
+      <c r="J116" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:N100"/>
+  <autoFilter ref="A1:N113"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -5022,10 +6569,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5034,7 +6581,7 @@
     <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -5044,8 +6591,11 @@
       <c r="C1" s="20" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5056,7 +6606,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5067,7 +6617,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5078,7 +6628,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5089,7 +6639,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5100,70 +6650,84 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C7" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>83</v>
+      </c>
+      <c r="D8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C9" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C10" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C11" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C12" t="s">
         <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update status and change dates
</commit_message>
<xml_diff>
--- a/docs/PM-1 Project Management/PM-1.2 Plans/PM-1.2.1 Project Plan/vms_implementation_plan_v0.1a.xlsx
+++ b/docs/PM-1 Project Management/PM-1.2 Plans/PM-1.2.1 Project Plan/vms_implementation_plan_v0.1a.xlsx
@@ -13,7 +13,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$51</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tasks!$A$1:$N$113</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tasks!$A$1:$N$116</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="162">
   <si>
     <t>No</t>
   </si>
@@ -681,6 +681,9 @@
   </si>
   <si>
     <t>Dio, Jifa</t>
+  </si>
+  <si>
+    <t>Find code to do zip utility</t>
   </si>
 </sst>
 </file>
@@ -844,8 +847,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="527">
+  <cellStyleXfs count="533">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1408,7 +1417,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="527">
+  <cellStyles count="533">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1672,6 +1681,9 @@
     <cellStyle name="Followed Hyperlink" xfId="522" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="524" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="526" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="528" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="530" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="532" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1935,6 +1947,9 @@
     <cellStyle name="Hyperlink" xfId="521" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="523" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="525" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="527" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="529" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="531" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3017,13 +3032,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N116"/>
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:N117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C93" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C112" sqref="C112"/>
+      <selection pane="bottomRight" activeCell="G118" sqref="G118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3087,7 +3103,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" hidden="1">
       <c r="B2" t="s">
         <v>79</v>
       </c>
@@ -3122,7 +3138,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" hidden="1">
       <c r="B3" t="s">
         <v>79</v>
       </c>
@@ -3157,7 +3173,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" hidden="1">
       <c r="B4" t="s">
         <v>79</v>
       </c>
@@ -3192,7 +3208,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" hidden="1">
       <c r="B5" t="s">
         <v>81</v>
       </c>
@@ -3230,7 +3246,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" hidden="1">
       <c r="B6" t="s">
         <v>79</v>
       </c>
@@ -3288,7 +3304,7 @@
         <v>40901</v>
       </c>
       <c r="I7" s="18">
-        <v>40901</v>
+        <v>40903</v>
       </c>
       <c r="J7" t="s">
         <v>39</v>
@@ -3326,7 +3342,7 @@
         <v>40902</v>
       </c>
       <c r="I8" s="18">
-        <v>40902</v>
+        <v>40903</v>
       </c>
       <c r="J8" t="s">
         <v>39</v>
@@ -3364,7 +3380,7 @@
         <v>40901</v>
       </c>
       <c r="I9" s="18">
-        <v>40901</v>
+        <v>40903</v>
       </c>
       <c r="J9" t="s">
         <v>39</v>
@@ -3402,7 +3418,7 @@
         <v>40902</v>
       </c>
       <c r="I10" s="18">
-        <v>40902</v>
+        <v>40903</v>
       </c>
       <c r="J10" t="s">
         <v>39</v>
@@ -3440,7 +3456,7 @@
         <v>40901</v>
       </c>
       <c r="I11" s="18">
-        <v>40902</v>
+        <v>40903</v>
       </c>
       <c r="J11" t="s">
         <v>9</v>
@@ -3478,7 +3494,7 @@
         <v>40902</v>
       </c>
       <c r="I12" s="18">
-        <v>40902</v>
+        <v>40903</v>
       </c>
       <c r="J12" t="s">
         <v>9</v>
@@ -3493,7 +3509,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" hidden="1">
       <c r="B13" t="s">
         <v>95</v>
       </c>
@@ -3528,7 +3544,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" hidden="1">
       <c r="B14" t="s">
         <v>97</v>
       </c>
@@ -3599,7 +3615,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" hidden="1">
       <c r="B16" t="s">
         <v>79</v>
       </c>
@@ -6486,7 +6502,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="114" spans="2:10">
+    <row r="114" spans="2:10" hidden="1">
       <c r="B114" t="s">
         <v>101</v>
       </c>
@@ -6532,7 +6548,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="116" spans="2:10">
+    <row r="116" spans="2:10" hidden="1">
       <c r="C116" t="s">
         <v>148</v>
       </c>
@@ -6555,8 +6571,29 @@
         <v>6</v>
       </c>
     </row>
+    <row r="117" spans="2:10">
+      <c r="C117" t="s">
+        <v>161</v>
+      </c>
+      <c r="D117" t="s">
+        <v>92</v>
+      </c>
+      <c r="E117" t="s">
+        <v>103</v>
+      </c>
+      <c r="G117" s="19" t="s">
+        <v>87</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:N113"/>
+  <autoFilter ref="A1:N116">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="New"/>
+        <filter val="WIP"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>